<commit_message>
Add Filtering by Versions
</commit_message>
<xml_diff>
--- a/Data/2017_11_14/output_py.xlsx
+++ b/Data/2017_11_14/output_py.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="652">
   <si>
     <t>Store</t>
   </si>
@@ -57,109 +57,142 @@
     <t>Appbot</t>
   </si>
   <si>
-    <t>Had to Delete App, then Reinstall to Fix. Review as of 11/14/17 @ 4:55 PM EST_x000D__x000D_Unfortunately, the only way to get Firefox to work was to uninstall it and reinstall it.  Unfortunately, lost some of my Bookmarks that I added on my iPad and that would never Sync to my Firefox Bookmarks across all used platforms - PC, iMac, etc.  Ah, the joys of technology!  Wish I could give it all up!!!_x000D__x000D_Review as of 11/14/17 around 4:00 PM EST_x000D__x000D_Cannot Open After Update_x000D__x000D_Have latest iOS 11.11.1 on my iPad Air 2.  This latest Firefox Update doesnÛªt even open.  Crashes every single time.  Please help!  Thanks!</t>
-  </si>
-  <si>
-    <t>Echt een aanrader. Werkt super goed_ÙÔ</t>
-  </si>
-  <si>
-    <t>Best browser option, could use some improvements on the margins. Definitely the best web browser IÛªve found for iPad. I basically use my iPad as a laptop and thus use the Firefox app as a desktop browser. For the most part, it serves this purpose well. The browser is easy to use, it loads pages quickly, and itÛªs (admittedly limited) settings options are simple and straight-forward. _x000D__x000D_However there are a few settings that could be changed to improve the user experience:_x000D__x000D_1. Allow users to make desktop mode the default setting._x000D__x000D_2. Allow users to set a default start-up page instead of opening all the tabs that were left open during the previous session._x000D__x000D_3. Allow users to change the order of sites on the bookmarks and top sites pages._x000D__x000D_4. Allow users to create folders or categories in the bookmarks menu</t>
-  </si>
-  <si>
-    <t>DerniÌ¬re mise ÌÊ jour quasi parfaite !. Enfin !!! Enfin Firefox est quasi aussi fluide que Safari ! JÛªaime beaucoup la philosophie de Mozilla mais ces derniers temps jÛªavais de plus en plus de mal a utiliser leur navigateur au profit de Safari..._x000D_Et avec cette mise ÌÊ jour, on a enfin quelque chose de fluide, rapide sans lags ! On peut enfin avoir la liste des onglets ouverts sur la barre du bas et non plus en haut (difficile dÛªaccÌ¬s sur un modÌ¬le Plus). JÛªaime beaucoup la nouvelle interface photon. Bref une rÌ©ussite._x000D__x000D_Le seul petit point que jÛªai ÌÊ reprocher cÛªest que pour ouvrir un onglet on est obligÌ© dÛªaller sur la liste des onglets et dÛªappuyer sur åÇ + åÈ, cÛªÌ©tait un peu plus rapide sur lÛªancienne version avec le menu rapide au milieu de la barre dÛªinterface du bas.</t>
-  </si>
-  <si>
-    <t>Version 10.1 is Great. Version 10.1 (Nov 2017) is a big improvement for usability and stability. The new top and bottom bars are perfect. The new buttons are in great positions for me. _x000D__x000D_Firefox for iOS is a stable browser, does everything chrome does. I trust Firefox more than Chrome. DonÛªt give all your personal data to Google. _x000D__x000D_ThereÛªs still a minor issue with  clicking some picture links.</t>
-  </si>
-  <si>
-    <t>Probleme in aktueller Version. Unter iOS 10.3.3 laden im privaten Modus fast keine Webseiten. URL copy in FF funktioniert nicht. _x000D_Fehlerbehebung dringend notwendig._x000D_Die Datenschutz-Richtlinine ist ( analog Desktop Version) leider fraglich. Sehr schade.</t>
-  </si>
-  <si>
-    <t>After long time writes  review. It need more works but itÛªs getting better._x000D_I like the new looks and performance and looking forward to see new quantum... .</t>
+    <t>Had to Delete App, then Reinstall to Fix. Review as of 11/14/17 @ 4:55 PM EST
+Unfortunately, the only way to get Firefox to work was to uninstall it and reinstall it.  Unfortunately, lost some of my Bookmarks that I added on my iPad and that would never Sync to my Firefox Bookmarks across all used platforms - PC, iMac, etc.  Ah, the joys of technology!  Wish I could give it all up!!!
+Review as of 11/14/17 around 4:00 PM EST
+Cannot Open After Update
+Have latest iOS 11.11.1 on my iPad Air 2.  This latest Firefox Update doesn’t even open.  Crashes every single time.  Please help!  Thanks!</t>
+  </si>
+  <si>
+    <t>Echt een aanrader. Werkt super goed👍</t>
+  </si>
+  <si>
+    <t>Best browser option, could use some improvements on the margins. Definitely the best web browser I’ve found for iPad. I basically use my iPad as a laptop and thus use the Firefox app as a desktop browser. For the most part, it serves this purpose well. The browser is easy to use, it loads pages quickly, and it’s (admittedly limited) settings options are simple and straight-forward. 
+However there are a few settings that could be changed to improve the user experience:
+1. Allow users to make desktop mode the default setting.
+2. Allow users to set a default start-up page instead of opening all the tabs that were left open during the previous session.
+3. Allow users to change the order of sites on the bookmarks and top sites pages.
+4. Allow users to create folders or categories in the bookmarks menu</t>
+  </si>
+  <si>
+    <t>Dernière mise à jour quasi parfaite !. Enfin !!! Enfin Firefox est quasi aussi fluide que Safari ! J’aime beaucoup la philosophie de Mozilla mais ces derniers temps j’avais de plus en plus de mal a utiliser leur navigateur au profit de Safari...
+Et avec cette mise à jour, on a enfin quelque chose de fluide, rapide sans lags ! On peut enfin avoir la liste des onglets ouverts sur la barre du bas et non plus en haut (difficile d’accès sur un modèle Plus). J’aime beaucoup la nouvelle interface photon. Bref une réussite.
+Le seul petit point que j’ai à reprocher c’est que pour ouvrir un onglet on est obligé d’aller sur la liste des onglets et d’appuyer sur « + », c’était un peu plus rapide sur l’ancienne version avec le menu rapide au milieu de la barre d’interface du bas.</t>
+  </si>
+  <si>
+    <t>Version 10.1 is Great. Version 10.1 (Nov 2017) is a big improvement for usability and stability. The new top and bottom bars are perfect. The new buttons are in great positions for me. 
+Firefox for iOS is a stable browser, does everything chrome does. I trust Firefox more than Chrome. Don’t give all your personal data to Google. 
+There’s still a minor issue with  clicking some picture links.</t>
+  </si>
+  <si>
+    <t>Probleme in aktueller Version. Unter iOS 10.3.3 laden im privaten Modus fast keine Webseiten. URL copy in FF funktioniert nicht. 
+Fehlerbehebung dringend notwendig.
+Die Datenschutz-Richtlinine ist ( analog Desktop Version) leider fraglich. Sehr schade.</t>
+  </si>
+  <si>
+    <t>After long time writes  review. It need more works but it’s getting better.
+I like the new looks and performance and looking forward to see new quantum... .</t>
   </si>
   <si>
     <t>Design. The design is awful.</t>
   </si>
   <si>
-    <t>Super. Die neue Ordnung. Erst Ì_berrascht, aber sie ist genau Richtig. Die neuen Funktionen   wie am GerÌ_t senden, habe ich bisher immer per Email gemacht so geht es einfach und schnell.</t>
+    <t>Super. Die neue Ordnung. Erst überrascht, aber sie ist genau Richtig. Die neuen Funktionen   wie am Gerät senden, habe ich bisher immer per Email gemacht so geht es einfach und schnell.</t>
   </si>
   <si>
     <t>Heyy. That's pretty good</t>
   </si>
   <si>
-    <t>____Û__. ____Û___¡_ÈÎ____ â_¡_¼, ___µ â__Û_____á_üâ, __â_¼ÛÜ___¡_µâ _±ÜâÛ__.</t>
-  </si>
-  <si>
-    <t>IcÌ«ne. Trop mimi ce nouvel icÌ«ne renard _Ù___ÙÕ¥ jÛªadore !</t>
+    <t>норм. нормально так, не тормозит, открывается быстро.</t>
+  </si>
+  <si>
+    <t>Icône. Trop mimi ce nouvel icône renard 🦊💕 j’adore !</t>
   </si>
   <si>
     <t>Ok. It will be awesome if you add chromecast on YouTube</t>
   </si>
   <si>
-    <t>Promising beta. I like Firefox sync and the new UI is nicely polished. _x000D__x000D_Fans of ad blockers will be disappointed that even Mozilla's own Focus is not supported.</t>
+    <t>Promising beta. I like Firefox sync and the new UI is nicely polished. 
+Fans of ad blockers will be disappointed that even Mozilla's own Focus is not supported.</t>
   </si>
   <si>
     <t>Endlich alles gut. Version 10.1. Gutes Update.</t>
   </si>
   <si>
-    <t>Bonne appli. Manque juste un gestionnaire de tÌ©lÌ©chargement mais tenant que lÛªiPhone dispose dÛªun gestionnaire de fichier._x000D_Pour info pour ceux qui ne savent pas, Firefox Focus est un autre navigateur constamment en navigation privÌ©e et plus lÌ©ger !_x000D_A dÌ©couvrir.</t>
-  </si>
-  <si>
-    <t>El mejor navegador. La aplicaciÌ_n que mÌÁs uso desde hace mÌÁs de 10 aÌ±os en windows, linux y recientemente en iphone y ipad tambiÌ©n. Sincroniza los complementos, las preferencias, los marcadores o lo que elijas, entre dispositivos. Ahora con interfaz mejorado</t>
+    <t>Bonne appli. Manque juste un gestionnaire de téléchargement mais tenant que l’iPhone dispose d’un gestionnaire de fichier.
+Pour info pour ceux qui ne savent pas, Firefox Focus est un autre navigateur constamment en navigation privée et plus léger !
+A découvrir.</t>
+  </si>
+  <si>
+    <t>El mejor navegador. La aplicación que más uso desde hace más de 10 años en windows, linux y recientemente en iphone y ipad también. Sincroniza los complementos, las preferencias, los marcadores o lo que elijas, entre dispositivos. Ahora con interfaz mejorado</t>
   </si>
   <si>
     <t>Comebtario. Creo que les Debo  disculpas espero y medissculpen undia nunca e tenido propblemas conesta aplicasion nose como esplicarlo pero es al go especial para mi</t>
   </si>
   <si>
-    <t>No add ons. IÛªd love to use Firefox with some ad blockers but nope.</t>
+    <t>No add ons. I’d love to use Firefox with some ad blockers but nope.</t>
   </si>
   <si>
     <t>Back to Chrome. I cannot upgrade to iOS 10, so I will not use it anymore</t>
   </si>
   <si>
-    <t>Trust Firefox Than Chrome. Google is like a creepy stalker following everything we do everywhere. So I prefer anything but Google search engine. But this latest update from Firefox is confusing. I donÛªt like it at all. Thus only 3 stars now.</t>
-  </si>
-  <si>
-    <t>»¬¡Ó_¥±Û ÎÎ_« â÷ÛÒø. ÂüÊÏ_Ó __¬¡_ü¡ü¡ ÂÁÂ_÷Ù_ ä_Ó¥÷_Î ¥«ãÊ_Ä¡ªÛ¡ öã¡Û ¤ÎÒÊ±«¤Û ¡ÏÐÁ¡ªÎ áü_÷ã »¬¡Ó__ãÊãÛ Ä_ã _¤¥÷_Î _«ÑÂ_÷ãÏ ¢ÜÛ_Ä¡ªÎ âÂÎÎ_Â_Ó ¡ü_ÊÒ¡Ê__ÊÐö_Ó¡ ¥÷ã ¥Êö÷_ö_Ó_Î Ñ Ð«ãÏ üã¡ãáµ__ÓÎÁÏÙÂüäüÒø</t>
-  </si>
-  <si>
-    <t>UPDate¤âãÙâäÉ»£Ù. ¾Ñ©Ñâ</t>
-  </si>
-  <si>
-    <t>Sharing and Reloading. I don't see the importance of reloading enough to place a big button in the middle bar menu._x000D_It should be the complex sharing shortcut instead!_x000D_Why place it awkwardly on top as 3 dots?</t>
-  </si>
-  <si>
-    <t>øáÑ¨ø Ê¨__¨¾÷øü»¾Ô ¨_Ñ_Ù. É¦ÈÐÄ_¾Î¼´__ã_Î_ ¾÷øø Ê¨__¨¼ ¾Ê_¾ÏÂ¾_Á¾ÏäÓ¬¥_ÛâüÛÝ«¾_Á¼¼¼ÓÑ_Ù_Ïü¼üÛü»__ÙÓÙ¾µ¤öª¬_Î¾öÔüÎ¾ÏÝ¾äÒ_Û_øÈ¦¾Ñ¦ÏÛ_ø Ê¾öÐ¾÷ø¾Îà¼_¤£ÓÛâ</t>
+    <t>Trust Firefox Than Chrome. Google is like a creepy stalker following everything we do everywhere. So I prefer anything but Google search engine. But this latest update from Firefox is confusing. I don’t like it at all. Thus only 3 stars now.</t>
+  </si>
+  <si>
+    <t>모바일앱은 파폭이 나은듯. 문제는 즐겨찾기인데 크롬처럼 평범하게 해도될것같은데 누가 만든건지 개떡같음 그래도 모바일버전은 탭을 큼직하게 보여줘서 좋은것같음 사파리는 참고쓰려고했는데 하도 할수있는게 없어서 인터넷익스플로러급인듯</t>
+  </si>
+  <si>
+    <t>UPDateでやたら遅くなった. 早くしろ</t>
+  </si>
+  <si>
+    <t>Sharing and Reloading. I don't see the importance of reloading enough to place a big button in the middle bar menu.
+It should be the complex sharing shortcut instead!
+Why place it awkwardly on top as 3 dots?</t>
+  </si>
+  <si>
+    <t>请问密码设置是个摆设吗？. 其他都挺好的，但是密码设置了根本没有用啊。一直没人反应吗？作为一个非原生浏览器，我希望打开软件时需要密码或是指纹解锁。</t>
   </si>
   <si>
     <t>Great job. Love the new Photon design and simple the best browser be it desktop or mobile.</t>
   </si>
   <si>
-    <t>Great browser. Looking and working fine _ÙÔ</t>
-  </si>
-  <si>
-    <t>So now itÛªs gone totally bad.... Before the update where they added the ÛÏphotonÛ look, it was great. Now it looks and acts like those crappy browsers (ex. Microsoft edge, Safari, etc.), and the so called tracking protection. It protects you from nothing, all they do is send the site a donÛªt track message, and most sites donÛªt know how to receive it, and if they do, they donÛªt care! BUT google they give your history ON Purpose for some research or something!! The tracking protection seems to be a tracking system in disguise, plus it freezes and crashes every time I open a new tab. Before the updates where they did this it was good. Now itÛªs totally bad.</t>
-  </si>
-  <si>
-    <t>Going down hill. I did not ask for and do not want this new "pocket" feature which is a third party website service anyway._x000D_Can someone tell me how to get rid of this new feature._x000D_Perhaps its time to move on from firefox.</t>
+    <t>Great browser. Looking and working fine 👍</t>
+  </si>
+  <si>
+    <t>So now it’s gone totally bad.... Before the update where they added the “photon” look, it was great. Now it looks and acts like those crappy browsers (ex. Microsoft edge, Safari, etc.), and the so called tracking protection. It protects you from nothing, all they do is send the site a don’t track message, and most sites don’t know how to receive it, and if they do, they don’t care! BUT google they give your history ON Purpose for some research or something!! The tracking protection seems to be a tracking system in disguise, plus it freezes and crashes every time I open a new tab. Before the updates where they did this it was good. Now it’s totally bad.</t>
+  </si>
+  <si>
+    <t>Going down hill. I did not ask for and do not want this new "pocket" feature which is a third party website service anyway.
+Can someone tell me how to get rid of this new feature.
+Perhaps its time to move on from firefox.</t>
   </si>
   <si>
     <t>Request desktop != open app. Wow. Enough said. What the ef Firefox</t>
   </si>
   <si>
-    <t>Locks up / slow. App has started to lock up a lot now. _x000D__x000D_The new menu feels really weird compared to the last one too, could just take some getting used to though. _x000D__x000D_The QR bar in the top right is also really annoying as I will never use it, so it would be nice to be able to remove it or replace it with something else.</t>
-  </si>
-  <si>
-    <t>Wird immer schlechter. Seit Umstellung auf ios11 bleibt die seite ne kurzen Moment Ì¦fters hÌ_ngen. _x000D_Auf ios 10 lief alles wunderbar _x000D__x000D_Bitte um update, danke._x000D__x000D_Dann gibt es auch 5 sterneÏÎü</t>
+    <t>Locks up / slow. App has started to lock up a lot now. 
+The new menu feels really weird compared to the last one too, could just take some getting used to though. 
+The QR bar in the top right is also really annoying as I will never use it, so it would be nice to be able to remove it or replace it with something else.</t>
+  </si>
+  <si>
+    <t>Wird immer schlechter. Seit Umstellung auf ios11 bleibt die seite ne kurzen Moment öfters hängen. 
+Auf ios 10 lief alles wunderbar 
+Bitte um update, danke.
+Dann gibt es auch 5 sterne✌️</t>
   </si>
   <si>
     <t>It's Firefox. The best of its kind</t>
   </si>
   <si>
-    <t>Firefox is the Best App  - 5 STARS. Firefox is the best ! App - itÛªs  Fast _x000D_Reliable - and I rate 5 stars plus extra - fantastic app I enjoy using this app because itÛªs so good !_x000D_Thank you to the team that designed this wonderful app !_x000D_ItÛªs great Firefox design !_x000D_Sidney-007_x000D_Electronic engineer</t>
-  </si>
-  <si>
-    <t>Pages donÛªt load fully. Pages only load at the top way to often. Once you scroll down there is nothing to see.  It cant be fixed by refreshing. Only by closing out and opening up on a new page or even closing the app out completely. Wish I hadn't of updated.</t>
+    <t>Firefox is the Best App  - 5 STARS. Firefox is the best ! App - it’s  Fast 
+Reliable - and I rate 5 stars plus extra - fantastic app I enjoy using this app because it’s so good !
+Thank you to the team that designed this wonderful app !
+It’s great Firefox design !
+Sidney-007
+Electronic engineer</t>
+  </si>
+  <si>
+    <t>Pages don’t load fully. Pages only load at the top way to often. Once you scroll down there is nothing to see.  It cant be fixed by refreshing. Only by closing out and opening up on a new page or even closing the app out completely. Wish I hadn't of updated.</t>
   </si>
   <si>
     <t>Go Firefox!. The only thing I really miss with Firefox on iPad is an option to change the order of top sites and bookmarks. Would be great to just tap/press and drag to arrange in whatever order you want.</t>
@@ -174,10 +207,17 @@
     <t>Love the new version. I'm impressed. The new version has a sleek new look and it's even faster to load than the old version. Love the new firefox app icon with black background. I'm still getting use to the rearranged menu and icon placements. Sadly the ability to edit and arrange our bookmarks in folders is still lacking and the Pin to tiles is still not great. App won't let me pin two the same website but with diferent content. Can I make a request to have a clear history option on the history tab for easy access.</t>
   </si>
   <si>
-    <t>ªã_ÊÉÄÈ¦. üÎ¾ÏÝøÈ´Ó¬ªã_ÊÉÄÈ¦</t>
-  </si>
-  <si>
-    <t>New look is great!. I'd like to see:_x000D_-adblocker_x000D_-content settings to auto delete cookies_x000D_-bookmarks that are easier to use, make them into big buttons like the recent history ones_x000D_-the browser needs to be faster_x000D_-it rarely crashes_x000D_-the reader view has lots of options_x000D_-change addons to extensions and make them available on iOS</t>
+    <t>附加元件. 希望可以用附加元件</t>
+  </si>
+  <si>
+    <t>New look is great!. I'd like to see:
+-adblocker
+-content settings to auto delete cookies
+-bookmarks that are easier to use, make them into big buttons like the recent history ones
+-the browser needs to be faster
+-it rarely crashes
+-the reader view has lots of options
+-change addons to extensions and make them available on iOS</t>
   </si>
   <si>
     <t>Editing bookmarks. I wish that I could rename the bookmarks and can move them around into an order that I prefer</t>
@@ -186,16 +226,20 @@
     <t>Love the new Design. The new design is great.  Was pleasantly surprised when I noticed the night mode option, thanks so much for including that.  Makes me wish the Mozilla phone had worked out.</t>
   </si>
   <si>
-    <t>Photon is Amazing. The new ÛÏPhotonÛ layout is perfect. The old style was passable but still felt clunky. But this new style just seems to flow so much better and smoother. The button layout is better suited for mobile as is the new No Images feature to help with data usage. Keep it up moz://a!</t>
-  </si>
-  <si>
-    <t>Ugliest icon I ever seen. What is this the 80Ûªs ?. Ugliest icon I ever seen. What is this the 80Ûªs ?</t>
-  </si>
-  <si>
-    <t>All my bookmarks vanished, ugly new logo. _ÙÕ©. After installing latest update 'Photon', every single bookmark and saved speed dial tile has absolutely VANISHED. There is no way for me to get back to my old bookmarks. Extremely disapointed, this was my main browser on mobile and now all the websites and links I had been saving since the app was released are totally and absolutely GONE. My bookmarks are now EMPTY._x000D__x000D_New logo is absolutely ridiculously oversaturated and dark. What were they thinking?_x000D__x000D_Shame on the mobile team.</t>
-  </si>
-  <si>
-    <t>Parfait. Clairement le meilleur navigateur sur iOS._x000D_IntÌ©gration de plusieurs moteurs de recherche, rapiditÌ©, navigation privÌ©e, des paramÌ¬tres complets et efficaces. _x000D_Rien ÌÊ redire. _ÙÔ_ÙÈ_ÙÔ_ÙÈ_ÙÔ_ÙÈ</t>
+    <t>Photon is Amazing. The new “Photon” layout is perfect. The old style was passable but still felt clunky. But this new style just seems to flow so much better and smoother. The button layout is better suited for mobile as is the new No Images feature to help with data usage. Keep it up moz://a!</t>
+  </si>
+  <si>
+    <t>Ugliest icon I ever seen. What is this the 80’s ?. Ugliest icon I ever seen. What is this the 80’s ?</t>
+  </si>
+  <si>
+    <t>All my bookmarks vanished, ugly new logo. 💩. After installing latest update 'Photon', every single bookmark and saved speed dial tile has absolutely VANISHED. There is no way for me to get back to my old bookmarks. Extremely disapointed, this was my main browser on mobile and now all the websites and links I had been saving since the app was released are totally and absolutely GONE. My bookmarks are now EMPTY.
+New logo is absolutely ridiculously oversaturated and dark. What were they thinking?
+Shame on the mobile team.</t>
+  </si>
+  <si>
+    <t>Parfait. Clairement le meilleur navigateur sur iOS.
+Intégration de plusieurs moteurs de recherche, rapidité, navigation privée, des paramètres complets et efficaces. 
+Rien à redire. 👏🏻👏🏻👏🏻</t>
   </si>
   <si>
     <t>Not working. Look out if you have an iPad pro this update doesn't work</t>
@@ -204,16 +248,19 @@
     <t>Dead on arrival after update. Running iOS 10.  Updated Firefox - opens and immediately freezes.  Nothing works, even after a reboot.   I depend on Firefox daily.  I hope they get this fixed fast.</t>
   </si>
   <si>
-    <t>_Ù_È__É____ _«_ü_á_¡____. _¢_µ_____¡ _À___È___¼_¡ ___¡___µÛÉÄ. __µ_____á_____¦____ _À_µÛ_µâ_¡_¼_ü___¡âÎ â_¡_±Ü._x000D___µâ _±_È___¼_üÛ____ä_ü_¼_¡ _±_¡_____µÛ____.</t>
-  </si>
-  <si>
-    <t>Manca la visualizzazione della barra segnalibri!. L'accesso ai segnalibri Ì¬ lento: se ci fosse la possibilitÌÊ di visualizzare la barra dei segnalibri come nella versione desktop... quinta stella!</t>
-  </si>
-  <si>
-    <t>Better on iPad. I'd give the iPhone version 2.5 stars. I'd prefer actual tabs, but this is still better than Firefox Focus.on the iPad pro, it's probably 4 or 4.5 stars. That implementation is excellent and I wish they'd do the same on the 6+ (at least do it in landscape mode)._x000D__x000D_I'll probably stick to dolphin on my phone and this on my iPad._x000D__x000D_Edit: Still like iPad version, but why doesn't focus go to the URL text area when a tab is opened?  Makes no sense (though I've seen the same problem in other iOS apps)</t>
-  </si>
-  <si>
-    <t>Open link new tab. Click on link and select open new tab... opens tab but in the background. So yet another click on the tab youÛªve just asked it to open. Back to safari until this is sorted.</t>
+    <t>Плохой дизайн. Темная полоска наверху. Невозможно перетаскивать табы.
+Нет блокировщика баннеров.</t>
+  </si>
+  <si>
+    <t>Manca la visualizzazione della barra segnalibri!. L'accesso ai segnalibri è lento: se ci fosse la possibilità di visualizzare la barra dei segnalibri come nella versione desktop... quinta stella!</t>
+  </si>
+  <si>
+    <t>Better on iPad. I'd give the iPhone version 2.5 stars. I'd prefer actual tabs, but this is still better than Firefox Focus.on the iPad pro, it's probably 4 or 4.5 stars. That implementation is excellent and I wish they'd do the same on the 6+ (at least do it in landscape mode).
+I'll probably stick to dolphin on my phone and this on my iPad.
+Edit: Still like iPad version, but why doesn't focus go to the URL text area when a tab is opened?  Makes no sense (though I've seen the same problem in other iOS apps)</t>
+  </si>
+  <si>
+    <t>Open link new tab. Click on link and select open new tab... opens tab but in the background. So yet another click on the tab you’ve just asked it to open. Back to safari until this is sorted.</t>
   </si>
   <si>
     <t>bad. fck off. no private</t>
@@ -222,55 +269,60 @@
     <t>removed from dock. The new black background icon looks terrible with all of the other icons in my dock and on my homescreen. I had to put it in a folder.</t>
   </si>
   <si>
-    <t>Beats Opera Mini. Early days for me but this may be the answer in terms of reducing data usage when not on WiFi. IÛªm loyal to safari when on WiFi but had relied on opera mini when using data due to its data saving capabilities. But opera has gone totally down hill with compulsory news feed which, ironically, chews data. Firefox now lets you block images and so save a little data if youÛªre only wanting basic information. Easy to set-up and use, with ad-blocking features. Very promising.</t>
-  </si>
-  <si>
-    <t>Random emojis?. Good to see that 1Password integration works again - however, it looks like something is wrong with encoding since random emojis show up on random places on websites. _x000D_Also, a feature request: please incorporate Focus (or another content blocker).</t>
-  </si>
-  <si>
-    <t>Great! Best of all, not Google!. Good update with the latest version! _ÙÔ Best of all, Firefox isnÛªt Google!</t>
-  </si>
-  <si>
-    <t>La mejor. Para mÌ_ es la mejor apps de navegaciÌ_n en internet, sus ads son lo mÌÁximo y de gran ayuda.... gracias Mozilla Group... _ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ</t>
+    <t>Beats Opera Mini. Early days for me but this may be the answer in terms of reducing data usage when not on WiFi. I’m loyal to safari when on WiFi but had relied on opera mini when using data due to its data saving capabilities. But opera has gone totally down hill with compulsory news feed which, ironically, chews data. Firefox now lets you block images and so save a little data if you’re only wanting basic information. Easy to set-up and use, with ad-blocking features. Very promising.</t>
+  </si>
+  <si>
+    <t>Random emojis?. Good to see that 1Password integration works again - however, it looks like something is wrong with encoding since random emojis show up on random places on websites. 
+Also, a feature request: please incorporate Focus (or another content blocker).</t>
+  </si>
+  <si>
+    <t>Great! Best of all, not Google!. Good update with the latest version! 👍 Best of all, Firefox isn’t Google!</t>
+  </si>
+  <si>
+    <t>La mejor. Para mí es la mejor apps de navegación en internet, sus ads son lo máximo y de gran ayuda.... gracias Mozilla Group... 🌟🌟🌟🌟🌟</t>
   </si>
   <si>
     <t>Fat. Slow. Jerky. Forgets. Low productivity.. There are probably new features I'll come to appreciate later, but not yet. Firefox update is so fat, it forgets a tab's setting just going to a different tab -- productivity is horrible. Jerky load. Just seems to hang ........  then continues. New look is obtuse. Now getting "unexpected error" that I never saw before. Yeah, and add some kind of rudimentary bookmark editing and grouping. Back to trying Google and Safari again (ugh).  Firefox still my favorite desktop browser.</t>
   </si>
   <si>
-    <t>_ÔÛ_¡Ä_á_µÛ ___µ _±_µ_á___À_¡_µ__!. _Õ___ü___¡___ü_µ, _ÀÛ_ü _À___À_¡_«_¡___ü_ü ___¡ ___ÀÛ_µ_«_µ_ÈÔ____Ä_ âÛ_¡___ü Ä, _±Û_¡Ä_á_µÛ _À___á_____È_µâ __â_¼ÛÜ___¡âÎ âÛ_¡___ü Ä  ___ÀÛ_µ_«_µ_ÈÔ____Ü___ü ã__Û___¡___ü âÛ_µ_±Ä_ä_ü___ü ___¡_¦_¡â_ü ____, _µ_È_ü â_¡_¼_¡ âÛ_¡___ü _¡ __â_¼ÛÜ_È_¡Î, â__ _±___ÈÎö_µ ___ü_¼_¡_¼_üÉ _«_µ__â___ü__ __ _±Û_¡Ä_á_µÛ_µ _ÀÛ___ü_á___µâ_ü ___µ_ÈÎ_á, _ÀÛ_ü_È___¦_µ___ü_µ ___µ _À___á_____È_µâ _á_¡_¼ÛÜâÎ âÛ_¡___ü Ä __Ü_á___¡__öÄ_ âÄ ã__Û__Ä. _Á___±â___µ______ __Ü ___üà_µ____ Ä_¦_µ ___µ _____¦_µâ_µ _«_µ_È_¡âÎ. _¢___ÈÎ_¼__ _À___È____âÎ_ _á_¡_¼ÛÜâÎ _±Û_¡Ä_á_µÛ. __â__ _ÀÛ__â__ _«ÜÛ_üä_¡!!!</t>
-  </si>
-  <si>
-    <t>â¢ÄÑÄ»â¢â_â_Ä_. â¢ÄÑÄ»â¢â_â_Ä_ÎÈÕÄªÄ_â_Ç»£_ªÓâÇÄÄâ_ããÛâ</t>
+    <t>Браузер не безопасен!. Внимание, при попадании на определённую страницу, браузер позволяет открывать страницу с определёнными формами требующими нажатия ОК, если такая страница открылась, то больше никаких действий в браузере произвести нельзя, приложение не позволяет закрыть страницу вызвавшую эту форму. Собственно вы ничего уже не можете сделать. Только полностью закрыть браузер. Это просто дырища!!!</t>
+  </si>
+  <si>
+    <t>アプリアイコン. アプリアイコンが黒ベースになってすごくカッコいい。</t>
   </si>
   <si>
     <t>WHERE ARE MY BOOKMARKS?!?. YEARS OF BOOKMARKS LOST!! I like Firefox but with the last update I no longer have my saved bookmarks. I tried the recovery on my laptop and still no luck!!! I had so many bookmarks saved and it's saddening to see them go which were very valuable links that I used for constant reference. Sad!!!!!</t>
   </si>
   <si>
-    <t>Olmas± gerektiÙi gibi. Sonunda yeni versiyonla olmas± gerektiÙi Ùeye dÌ¦nÌ_ÙtÌ_. Chrome un fazla yer kullanmas±ndan ve sevimsiz tasar±m±ndan kurtuldum. MasaÌ_stÌ_nde de kararl± sÌ_rÌ_m iÌ¤in 14 Kas±m ± bekliyorum. Denemeyen varsa kesinlikle bir Ùans vermeli.</t>
-  </si>
-  <si>
-    <t>Mozilla, please donÛªt go ÛÏChromeÛ on us!. As indicated in a previous post, the swaying toward GoogleÛªs Û÷Less is BestÛª look is not liked. I have been a devoted user of the Mozilla browser for 20+ years because it puts the relevant controls at my fingertips. This ÛÏminimalistÛ look gets away from MozillaÛªs browser purpose with each update, on all platforms (PC, Android, &amp; here for IOS). In particular with v10, the translucent appearance of the Settings menu is difficult. I am also not a fan of the Tabs being at the very top, I prefer them just above the page for quick reference to the PageÛªs Title, especially helpful to me when doing research on multiple sites - allowing quicker back &amp; forth switching,_x000D__x000D_Can you consider switches for the Translucency and the Tab Row positioning? I would be very grateful. I do like the Images off &amp; Night Modes choices - and the Sync &amp; Pocket functions are monumental and make my (need for info) life so much easier! _Ù÷Û_x000D__x000D_Thank you.</t>
-  </si>
-  <si>
-    <t>Tab-Leiste. Nach dem ÌÐffnen einer URL in neuem Tab sollte die Tab-Leiste angezeigt werden, ohne die ursprÌ_ngliche Seite in der Position (scrollen) verÌ_ndern zu mÌ_ssen.</t>
-  </si>
-  <si>
-    <t>Excellent browser! PW manager, not so much. With content blocking in effect in Firefox, it has risen to the top as my go-to browser. _x000D__x000D_Would give 5/5 if they could fix the password (log-in) manager, since it atm is broken, IMO. Fix that, and IÛªd gladly give 5 stars.</t>
-  </si>
-  <si>
-    <t>Adesso Ì¬ proprio il migliore. Con la nuova versione 10.0 ha rinforzato la sua leadership tra i browser per iOS. Io, con un "antiquato" iPhone 5 del 2012 vado come una scheggia! Attendo con ansia la nuova versione per desktop!</t>
-  </si>
-  <si>
-    <t>ü_ªÙø ¢_. ¾ÏäüÛ¼Ý¦_Çª_ãü_ªÙø ¢_ãÁ¾_¥¬÷_ã__÷_ÎÇÜ¾Ó_ÐãÛâ_x000D_Safariü_¾üÂ©_¾÷øøÈ´¬÷__ãÛâ</t>
-  </si>
-  <si>
-    <t>Mein Lieblingsbrowser. auf allen GerÌ_ten. Er wird immer besser.</t>
+    <t>Olması gerektiği gibi. Sonunda yeni versiyonla olması gerektiği şeye dönüştü. Chrome un fazla yer kullanmasından ve sevimsiz tasarımından kurtuldum. Masaüstünde de kararlı sürüm için 14 Kasım ı bekliyorum. Denemeyen varsa kesinlikle bir şans vermeli.</t>
+  </si>
+  <si>
+    <t>Mozilla, please don’t go “Chrome” on us!. As indicated in a previous post, the swaying toward Google’s ‘Less is Best’ look is not liked. I have been a devoted user of the Mozilla browser for 20+ years because it puts the relevant controls at my fingertips. This “minimalist” look gets away from Mozilla’s browser purpose with each update, on all platforms (PC, Android, &amp; here for IOS). In particular with v10, the translucent appearance of the Settings menu is difficult. I am also not a fan of the Tabs being at the very top, I prefer them just above the page for quick reference to the Page’s Title, especially helpful to me when doing research on multiple sites - allowing quicker back &amp; forth switching,
+Can you consider switches for the Translucency and the Tab Row positioning? I would be very grateful. I do like the Images off &amp; Night Modes choices - and the Sync &amp; Pocket functions are monumental and make my (need for info) life so much easier! 😀
+Thank you.</t>
+  </si>
+  <si>
+    <t>Tab-Leiste. Nach dem Öffnen einer URL in neuem Tab sollte die Tab-Leiste angezeigt werden, ohne die ursprüngliche Seite in der Position (scrollen) verändern zu müssen.</t>
+  </si>
+  <si>
+    <t>Excellent browser! PW manager, not so much. With content blocking in effect in Firefox, it has risen to the top as my go-to browser. 
+Would give 5/5 if they could fix the password (log-in) manager, since it atm is broken, IMO. Fix that, and I’d gladly give 5 stars.</t>
+  </si>
+  <si>
+    <t>Adesso è proprio il migliore. Con la nuova versione 10.0 ha rinforzato la sua leadership tra i browser per iOS. Io, con un "antiquato" iPhone 5 del 2012 vado come una scheggia! Attendo con ansia la nuova versione per desktop!</t>
+  </si>
+  <si>
+    <t>帳號密碼. 有一些網站的帳號密碼無法記住儲存，請改善。
+Safari上測試是可以記住的。</t>
+  </si>
+  <si>
+    <t>Mein Lieblingsbrowser. auf allen Geräten. Er wird immer besser.</t>
   </si>
   <si>
     <t>Firefox comes of age on iOS.. Adblocking finally comes to Firefox on iOS. Page loading and rendering is good. Great new layout. Can finally ditch safari.</t>
   </si>
   <si>
-    <t>ItÛªs Getting Better. ItÛªs nice to have a privacy conscious organization behind the browser. Though I wonder if Do Not Track really works or if, as the other reviewer said, itÛªs simply another means to track us by some websites. Mozilla please respond.</t>
+    <t>It’s Getting Better. It’s nice to have a privacy conscious organization behind the browser. Though I wonder if Do Not Track really works or if, as the other reviewer said, it’s simply another means to track us by some websites. Mozilla please respond.</t>
   </si>
   <si>
     <t>Worst Update in Years. I have fast fiber (125 Mbps) but this new Firefox takes 20 seconds to load the New York Times homepage! Can't fully render a Facebook page, stops halfway. Just a disaster in every use case. Sooooooo slow, like Edge slow. iPhone 6, iOS 11.1.1</t>
@@ -282,13 +334,16 @@
     <t>Force touch. Force touch feature enabled would be amazing</t>
   </si>
   <si>
-    <t xml:space="preserve">Ä_üÄ_ÀÓÝ_¾Ñ¤¥Î¢___. Ä_üÄ_ÀÓÝ_¾Ñ¤¥Î¢___ü¡ÀÄ¡±â_Óª¼ _Î¾Ð¡¥Î¢À÷ä_öÇöÇ¾ä__Î üÀ¨_»Ä__ÄÓ¬¼ </t>
-  </si>
-  <si>
-    <t>Muito bom. O design e as funÌ¤Ìµes excelentes._x000D_O meu navegador principal, sem duvidas.</t>
-  </si>
-  <si>
-    <t>Browser freezes a lot. Page loading issues.. Ever since ios 11.  _x000D__x000D_Are we ever going to get extensions?  Hello?_x000D__x000D_How about the taking our privacy seriously?   Hello?</t>
+    <t>能不能返回旧界面！！！. 能不能返回旧界面！！！不小心就点错了，新界面还特别别扭，再不修复只能弃用了</t>
+  </si>
+  <si>
+    <t>Muito bom. O design e as funções excelentes.
+O meu navegador principal, sem duvidas.</t>
+  </si>
+  <si>
+    <t>Browser freezes a lot. Page loading issues.. Ever since ios 11.  
+Are we ever going to get extensions?  Hello?
+How about the taking our privacy seriously?   Hello?</t>
   </si>
   <si>
     <t>Great Job Firefox!. You did a great job! and I think this is better than chrome and safari!</t>
@@ -297,16 +352,17 @@
     <t>Latest update the best version!!. Love the settings!!! Also love to speed and feel of the new firefox! Been an avid firefox user for years and i swear the browser just keeps getting better! Good job mozilla!</t>
   </si>
   <si>
-    <t>â¢ÄÄÄÑÄàÄ_ÄöÑÙâäÄ_â¡â_Ä_¤»»£Ù. â¢ÄÄÄÑÄàÄ_ÄöÑÙâäÄ_â¡â_Ä_Ç_±¾¥ÑÑ_ªÛâÄÔâ_ÄøÄ_ÄäÄ»âÈÄÄÄö¨ÄÁÄ_ÄÇââªÈÎ_¢¼»¨ÄÁÄ_ÄÇââ±__ÝâÒÛâÄÔâ_ÄøÄ_ÄäâÕÐÒ¥öÙÜ¬¾ÛãPC¤¢¼»Ñ_ªÎÛÐÒ¥öøââ__ÝâÒ_ÛâÁâÄâÒ¬Ä â_ÄöÑ_ÄàÄ»ÄÄ»Ä_Ñ_âÜ¨Ü»ÛÏ¾Ñ©¾_ÈÑ_</t>
-  </si>
-  <si>
-    <t>Nice update. Improvements needed. The v10 update is good. Tabs view icon is finally moved to the bottom bar; the weird margin to the right in reading mode is gone; UI overhaul is IMO good; extra love for the new icon. Now my go-to browser. _x000D__x000D_Some problems: 1. Why donÛªt use the icons provided by the sites in quick dials? For example, now Gmail in quick dials shows a Google icon, Instagram a blue icon (the legacy one) and Tumblr a green one. 2. The new tab icon is not in the same position as the tabs view icon. You tap the tabs view switch, the tabs view opens, but if you want to open a new tab youÛªd have to move your finger to the right a little. Not a big thing but can be annoying sometimes.</t>
+    <t>アップデートしたらログインできなくなった. アップデートしたらログインに失敗します。パスワードリセットのメールも登録確認のメールも届きません。パスワードを間違えたかと思いPCで確認しますが、間違えはありませんね。ちゃんとテストしてデリバリーしてるのかな〜早く治して</t>
+  </si>
+  <si>
+    <t>Nice update. Improvements needed. The v10 update is good. Tabs view icon is finally moved to the bottom bar; the weird margin to the right in reading mode is gone; UI overhaul is IMO good; extra love for the new icon. Now my go-to browser. 
+Some problems: 1. Why don’t use the icons provided by the sites in quick dials? For example, now Gmail in quick dials shows a Google icon, Instagram a blue icon (the legacy one) and Tumblr a green one. 2. The new tab icon is not in the same position as the tabs view icon. You tap the tabs view switch, the tabs view opens, but if you want to open a new tab you’d have to move your finger to the right a little. Not a big thing but can be annoying sometimes.</t>
   </si>
   <si>
     <t>Please bring back. Add cookies setting</t>
   </si>
   <si>
-    <t>Tabs. Das neue Design gefÌ_llt mir gut, aber wenn ich in die TabÌ_bersicht gehe fangen diese oben links an statt unten, das wechseln oder schlieÌÙen eines Tabs erfordert dann ein umgreifen.</t>
+    <t>Tabs. Das neue Design gefällt mir gut, aber wenn ich in die Tabübersicht gehe fangen diese oben links an statt unten, das wechseln oder schließen eines Tabs erfordert dann ein umgreifen.</t>
   </si>
   <si>
     <t>Love it. I mostly use it to view my Facebook groups because it loads the posts so much faster than safari. Safari is great for general web browsing though.</t>
@@ -318,16 +374,17 @@
     <t>Crash too mich. In IOS 11 for iphone 5S crash too much</t>
   </si>
   <si>
-    <t>Great update!. I enjoy the new interface, itÛªs just brilliant! Work with tabs is a real pleasure now. Many thanks!</t>
-  </si>
-  <si>
-    <t>Almost there.... The one feature I person still would love to have added is the ability to have Firefox launch into private mode and STAY in private mode (like an option to set it that way) so I don't have to switch after the fact or use 3D Touch to launch it that way. I don't want to have to set the option of not closing Private Tabs upon exit because, to me, that partially defeats the point of even using Private Tabs. They're supposed to leave no traces. The desktop version has this feature, iOS Safari has this feature, so why don't you guys do the same?_x000D__x000D_Another bug is the Night Mode. All Night Mode does is swap black and white for text and backgrounds. The bug is that if the page is already using a black background, Night Mode changes it to white, making the page NOT night-time-viewing friendly.  You need to add somw code to check what color the text and background already is before possibly changing anything because it may already be designed for night viewing.</t>
+    <t>Great update!. I enjoy the new interface, it’s just brilliant! Work with tabs is a real pleasure now. Many thanks!</t>
+  </si>
+  <si>
+    <t>Almost there.... The one feature I person still would love to have added is the ability to have Firefox launch into private mode and STAY in private mode (like an option to set it that way) so I don't have to switch after the fact or use 3D Touch to launch it that way. I don't want to have to set the option of not closing Private Tabs upon exit because, to me, that partially defeats the point of even using Private Tabs. They're supposed to leave no traces. The desktop version has this feature, iOS Safari has this feature, so why don't you guys do the same?
+Another bug is the Night Mode. All Night Mode does is swap black and white for text and backgrounds. The bug is that if the page is already using a black background, Night Mode changes it to white, making the page NOT night-time-viewing friendly.  You need to add somw code to check what color the text and background already is before possibly changing anything because it may already be designed for night viewing.</t>
   </si>
   <si>
     <t>Bookmarks. This update removed all the bookmarks that were synced with my desktop computer. Please fix this ASAP!</t>
   </si>
   <si>
-    <t>âÄ_À_üâ _ÀÛ_ü _______«_µ _±Ä_¼__. âÄ_À_üâ _ÀÛ_ü _______«_µ _±Ä_¼__ __ _¡_«Û_µ______ âÛ___¼_µ. _±_µ_üâ.</t>
+    <t>тупит при вводе букв. тупит при вводе букв в адресной строке. бесит.</t>
   </si>
   <si>
     <t>Bugs version 9.3. Embedded video player buttons are square shaped. The language within the options menu is different than the native language. Hope you fix this. Grtz</t>
@@ -336,13 +393,13 @@
     <t>Can't enter grades with latest update. Firefox will no longer let me enter student grades, how to go back to previous functional version?</t>
   </si>
   <si>
-    <t>New version glitchy.... The new version is glitchy compared to the last.  If you click a link and then close the linked page and then click a link within the original document again it wonÛªt open the links.</t>
+    <t>New version glitchy.... The new version is glitchy compared to the last.  If you click a link and then close the linked page and then click a link within the original document again it won’t open the links.</t>
   </si>
   <si>
     <t>Fat. Slow. Jerky. Forgets. Low productivity.. There are probably features I'll come to appreciate later, but not yet. Firefox update is so fat, it forgets a tab's setting just going to a different tab -- productivity is horrible. Jerky load. Just seems to hang ........  then continues. New look is obtuse. Yeah, and add some kind of rudimentary bookmark editing and grouping. Back to trying Google and Safari again.  Still my favorite desktop browser.</t>
   </si>
   <si>
-    <t>Greatest comeback. This is the best upgrade from Firefox. ItÛªs serious in being the toughest competition to Chrome. Very fast, clean design, and reliable. Great job Firefox team!</t>
+    <t>Greatest comeback. This is the best upgrade from Firefox. It’s serious in being the toughest competition to Chrome. Very fast, clean design, and reliable. Great job Firefox team!</t>
   </si>
   <si>
     <t>Extremely ugly new interface. The revised interface looks extremely ugly and does not fit to iOS at all.</t>
@@ -351,94 +408,114 @@
     <t>Aplikasi pintar. Mantap</t>
   </si>
   <si>
-    <t>Ì¤eviri. mutlaka Ì¤eviri Ì¦zelliÙi olmal±...</t>
-  </si>
-  <si>
-    <t>¾_¬¨_¡_Ñ_. _ÛüÈÁµÕÎöà¾¢¾Êà__ü¾Ð__À_À÷¾Ïä¾ø¾ÂÁ¾äÒ_Ûà»_¬_Ê___ÜäÁµ¢¾Û__öÉ_Ñ__Ù¾Ý«¾Ð¡_¾ä_üö¡¼ Ûâ</t>
+    <t>çeviri. mutlaka çeviri özelliği olmalı...</t>
+  </si>
+  <si>
+    <t>注定小众！. 开主页和切换标签不方便！还有每次打开自动加载之前页面怎么关闭？更新后找不到了。</t>
   </si>
   <si>
     <t>Getting there. But there is a bug that breaks the scrolling inertia and requires you to refresh the page to fix it.</t>
   </si>
   <si>
-    <t>Geht sicher noch besser. In der Version 10 ist die Benutzerfreundlichkeit ein klein wenig besser als auch schon, aber immer noch vÌ¦llig unbrauchbar. Dies ist vor allem bezogen auf die Lesezeichen. Diese lassen sich immer noch nicht bearbeiten (oder auf einem, nur den Entwicklern bekannten Weg), und es ist viel zu umstÌ_ndlich an das Lesezeichen-Menu zu gelangen.</t>
-  </si>
-  <si>
-    <t>Very Amazing. Very veryyy amazing tnx for big update relase _Ùª_ü_ÙÕÜ_ÙÎá</t>
+    <t>Geht sicher noch besser. In der Version 10 ist die Benutzerfreundlichkeit ein klein wenig besser als auch schon, aber immer noch völlig unbrauchbar. Dies ist vor allem bezogen auf die Lesezeichen. Diese lassen sich immer noch nicht bearbeiten (oder auf einem, nur den Entwicklern bekannten Weg), und es ist viel zu umständlich an das Lesezeichen-Menu zu gelangen.</t>
+  </si>
+  <si>
+    <t>Very Amazing. Very veryyy amazing tnx for big update relase 🙏❤️💋🌷</t>
   </si>
   <si>
     <t>Love the new interface. Much better than before . Good job guys</t>
   </si>
   <si>
-    <t>Get rid of pocket. I need a way to remove pocket from the screen. Please add something to settings I really donÛªt want this feature. Really.</t>
-  </si>
-  <si>
-    <t>Good update but.... Firefox has definitely improved its UI with the new update. I like the 'night mode' option that is much better now compared to the old that simply dimmed the brightness. There still needs to be a way to edit bookmarks and create folders to them... so that this iOS app is as useful as the desktop version._x000D__x000D_Issue (as of Nov 11 2017): Sometimes images get messed up when scrolling in night mode. _x000D__x000D_It would be really cool if the 'containers' feature on the desktop Firefox was added to iOS's version; that would really set iOS's Firefox apart as a great browser. I realize iOS has restrictions so addons might not be allowed by Apple in Firefox; although, those would be really cool too. I hope the developers will take note of this review and I appreciate the open-source and transparent philosophy Firefox has supported over the years.</t>
-  </si>
-  <si>
-    <t>Non salva le immagini. Ho dato una stella per far percepire il messaggio in fretta. Quando il nuovo IOS si Ì¬ aggiornato non fa piÌ_ salvare le immagini._x000D_Appena risolvete vi darÌ_ le meritatissime 5 stelle._x000D_Ho un Pad Air 2.</t>
+    <t>Get rid of pocket. I need a way to remove pocket from the screen. Please add something to settings I really don’t want this feature. Really.</t>
+  </si>
+  <si>
+    <t>Good update but.... Firefox has definitely improved its UI with the new update. I like the 'night mode' option that is much better now compared to the old that simply dimmed the brightness. There still needs to be a way to edit bookmarks and create folders to them... so that this iOS app is as useful as the desktop version.
+Issue (as of Nov 11 2017): Sometimes images get messed up when scrolling in night mode. 
+It would be really cool if the 'containers' feature on the desktop Firefox was added to iOS's version; that would really set iOS's Firefox apart as a great browser. I realize iOS has restrictions so addons might not be allowed by Apple in Firefox; although, those would be really cool too. I hope the developers will take note of this review and I appreciate the open-source and transparent philosophy Firefox has supported over the years.</t>
+  </si>
+  <si>
+    <t>Non salva le immagini. Ho dato una stella per far percepire il messaggio in fretta. Quando il nuovo IOS si è aggiornato non fa più salvare le immagini.
+Appena risolvete vi darò le meritatissime 5 stelle.
+Ho un Pad Air 2.</t>
   </si>
   <si>
     <t>Good update but.... Firefox has definitely improved its UI with the new update. I like the 'night mode' option that is much better now compared to the old that simply dimmed the brightness. There still needs to be a way to edit bookmarks and create folders to them... so that this iOS app is as useful as the desktop version. It would be really cool if the 'containers' feature on the desktop Firefox was added to iOS's version; that would really set iOS's Firefox apart as a great browser. I realize iOS has restrictions so addons might not be allowed by Apple in Firefox; although, those would be really cool too. I hope the developers will take note of this review and I appreciate the open-source and transparent philosophy Firefox has supported over the years.</t>
   </si>
   <si>
-    <t xml:space="preserve">¾¤_. _öÄ_üÛü»app»ã¦¾Ý«¾Ð¡_Ü_¾¢¼ Ý_¾Êà_ã¢Ïä__Î¾Îä¢Ïä_¾_ÕöÑÏ¬±_¥ü__Î_Ê»ã¦÷¼ ¢Ïä_...¾öÔ¾Û__ö¨ä¾_Õ_Ê_ã__¨_ÙÝÊü¼Àªü»Ñ¨¢÷öÊ¾_ä_ö__app¼ </t>
+    <t>吐槽. 很烦一个app突然更新之后换了图标的颜色，按颜色排列在屏幕上，你突然变了颜色...我怎么安排你的位置？因为这个问题删掉很多app了</t>
   </si>
   <si>
     <t>Adding block ads. Add ad-blocking utility loads the browser. Need to improve the performance and the speed of browsing the web. The management of the tag in the form of a larger window and can turn left or right to manage the tag. Can top up paws the screen to close the tag. Thank developers</t>
   </si>
   <si>
-    <t>Ü¥_ÏÎàã. È_Ý_¨â¢ÄÄÄÑÄàÄ_Äö¤Äàâ¦â_Ä_ø¬_ââäø»â__ÑÙÛâ_x000D__ÏÐÒÄ¢Ä_Ääâââ¢â_Äàâ¢øäøã¨¤ªÎÛÜ¥_ÏÎ¬_ââàãâö ¤ªÛâ</t>
-  </si>
-  <si>
-    <t>Ruim. Testei no computador e no celular pra substituir o Chrome que estÌÁ consumindo muita memÌ_ria. Mas o Firefox pro iPhone estÌÁ horrÌ_vel. NÌ£o renderiza as pÌÁginas, fica pÌÁginas em branco. Vou testar outros pra ver se ao menos funcionam, senÌ£o vou ter que ficar com o Chrome mesmo.</t>
-  </si>
-  <si>
-    <t>can not. âÀÄÐ¨ü__¾ÝÀöÎ¤»ãÛâ_x000D_ÄÐÄÄâøÄ_Ä_âøââü__¾ÝÀöÎà¼¾´»ãÛâ_x000D_ÈÐø_â_âÛâ_x000D__x000D_iPad Pro 10.5  iOS 11.1</t>
-  </si>
-  <si>
-    <t>Many improvements in Photon, lost a feature.. ItÛªs pretty decent for those who are skeptical. _x000D_But it gets rid of the ability to create a new tab and switch between private and normal browsing in 2 taps. Now you must open your list of tabs the old way. Hopefully they can bring that feature back soon. It was quite useful.</t>
+    <t>動作が重い. 今回のアップデートでデザインはとても良くなりました。
+夜間モードもアイデアは良いのですが、動作がとても重いようです。</t>
+  </si>
+  <si>
+    <t>Ruim. Testei no computador e no celular pra substituir o Chrome que está consumindo muita memória. Mas o Firefox pro iPhone está horrível. Não renderiza as páginas, fica páginas em branco. Vou testar outros pra ver se ao menos funcionam, senão vou ter que ficar com o Chrome mesmo.</t>
+  </si>
+  <si>
+    <t>can not. タブの並び替えができない。
+ブックマークも並び替えが出来ない。
+他はまあまあ。
+iPad Pro 10.5  iOS 11.1</t>
+  </si>
+  <si>
+    <t>Many improvements in Photon, lost a feature.. It’s pretty decent for those who are skeptical. 
+But it gets rid of the ability to create a new tab and switch between private and normal browsing in 2 taps. Now you must open your list of tabs the old way. Hopefully they can bring that feature back soon. It was quite useful.</t>
   </si>
   <si>
     <t>I hate black background. Good app but I hate that icon black background.</t>
   </si>
   <si>
-    <t>El mejor. Sencillamente el mejor navegador!! _x000D_Bloquea la publicidad y su velocidad es impresionante!</t>
-  </si>
-  <si>
-    <t>Ich mÌ¦chte Pocket nicht. Firefox ist fÌ_r mich eigentlich seit Jahren der Browser, da ich Mozilla verhÌ_ltnismÌ_ÌÙig vertraue! _x000D__x000D_Aber wenn ich jedes mal beim Ì¦ffnen neuer Tabs, mit dÌ_mlichen Mainstream-Nachrichten-Meldungen konfrontiert werde, finde ich das sehr unschÌ¦n._x000D__x000D_Ich hoffe ihr fÌ_gt die Einstellungs-Option ein, Pocket auszuschalten.</t>
-  </si>
-  <si>
-    <t>Great Alternative to safari, specially to windows users. I use Firefox every day on my windows laptop &amp; with Firefox new UI i feel i am more productive than ever now , specially with features like seeing tabs on my laptop or send tabs to_x000D__x000D_Keep the good work</t>
+    <t>El mejor. Sencillamente el mejor navegador!! 
+Bloquea la publicidad y su velocidad es impresionante!</t>
+  </si>
+  <si>
+    <t>Ich möchte Pocket nicht. Firefox ist für mich eigentlich seit Jahren der Browser, da ich Mozilla verhältnismäßig vertraue! 
+Aber wenn ich jedes mal beim öffnen neuer Tabs, mit dämlichen Mainstream-Nachrichten-Meldungen konfrontiert werde, finde ich das sehr unschön.
+Ich hoffe ihr fügt die Einstellungs-Option ein, Pocket auszuschalten.</t>
+  </si>
+  <si>
+    <t>Great Alternative to safari, specially to windows users. I use Firefox every day on my windows laptop &amp; with Firefox new UI i feel i am more productive than ever now , specially with features like seeing tabs on my laptop or send tabs to
+Keep the good work</t>
   </si>
   <si>
     <t>Smooth. Easy to use fast brower.</t>
   </si>
   <si>
-    <t>Focus on New Tab. When I press and hold on a link and select Open in New Tab_x000D_I EXPECT it to go to that Tab IMMEDIATELY._x000D_I should not have to Hunt around for the TAB !_x000D__x000D_The People who write the code , don't seem to understand how its supposed to work..._x000D__x000D_Google Chrome seems to have the same clueless ..._x000D__x000D_Thank God for Safari !   Its a Deal Braker for Firefox or Chrome and makes it an easy choice .  Safari gets me there quicker.</t>
-  </si>
-  <si>
-    <t>_Õ_µ ÉÄ_¦_µ _ü ÉÄ_¦_µ. __µ __ÉÛ_¡___â _È_____ü__Ü _ü _«_¡_¦_µ ___¡ Û__Äâ_µÛ  â______ _±Û_¡Ä_á_µÛ_¡ _á_¡__â_ü ___µ ______Ä â_µ_À_µÛÎ</t>
+    <t>Focus on New Tab. When I press and hold on a link and select Open in New Tab
+I EXPECT it to go to that Tab IMMEDIATELY.
+I should not have to Hunt around for the TAB !
+The People who write the code , don't seem to understand how its supposed to work...
+Google Chrome seems to have the same clueless ...
+Thank God for Safari !   Its a Deal Braker for Firefox or Chrome and makes it an easy choice .  Safari gets me there quicker.</t>
+  </si>
+  <si>
+    <t>Все хуже и хуже. Не сохраняются логины и даже на роутер с этого браузера зайти не могу теперь</t>
   </si>
   <si>
     <t>Stopped working in iPad 4, iOS10.3.3. This version doesn't open at all - not crash nor anything.</t>
   </si>
   <si>
-    <t>CadÌ» o leitor de QR Code?. Pra ficar perfeito, sÌ_ falta voltar o leitor de QR Code que havia antes dessa ultima versÌ£o!</t>
-  </si>
-  <si>
-    <t>CanÛªt zoom in!. Best feature of IOS is bench zoom why do you disable it? Uninstalled FF using Safari and Chrome.</t>
-  </si>
-  <si>
-    <t>Gorgeous. IÛªm really digging this new look. It might replace Safari on my phone now.</t>
-  </si>
-  <si>
-    <t>Ü¥_ÏÎàã. È_Ý_¨â¢ÄÄÄÑÄàÄ_Äö¤Äàâ¦â_Ä_ø¬_ââäø»â__ÑÙÛâ_x000D_ÙÊÑÜ¥_ÏÎàã¤ªÛâ</t>
-  </si>
-  <si>
-    <t>Excelente. Eu jÌÁ gostava dele e agora com a nova versÌ£o que trÌÁs os controles na parte debaixo do navegador ficou Ì_timo, muito mais prÌÁtico. EstÌÁ muito leve tambÌ©m Ì© com uma Ì_tima aparÌ»ncia.</t>
-  </si>
-  <si>
-    <t>_ÙÔ_. I had this quiz that I had to do in while in class. And I could not complete the quiz because the results button become unresponsive like other thing I do on Firefox on iOS._x000D_Deleted. Not taking another chance on this.</t>
+    <t>Cadê o leitor de QR Code?. Pra ficar perfeito, só falta voltar o leitor de QR Code que havia antes dessa ultima versão!</t>
+  </si>
+  <si>
+    <t>Can’t zoom in!. Best feature of IOS is bench zoom why do you disable it? Uninstalled FF using Safari and Chrome.</t>
+  </si>
+  <si>
+    <t>Gorgeous. I’m really digging this new look. It might replace Safari on my phone now.</t>
+  </si>
+  <si>
+    <t>動作が重い. 今回のアップデートでデザインはとても良くなりました。
+ただし動作が重いです。</t>
+  </si>
+  <si>
+    <t>Excelente. Eu já gostava dele e agora com a nova versão que trás os controles na parte debaixo do navegador ficou ótimo, muito mais prático. Está muito leve também é com uma ótima aparência.</t>
+  </si>
+  <si>
+    <t>👎. I had this quiz that I had to do in while in class. And I could not complete the quiz because the results button become unresponsive like other thing I do on Firefox on iOS.
+Deleted. Not taking another chance on this.</t>
   </si>
   <si>
     <t>Fat. Slow. Jerky. Forgets. Low productivity.. There are probably features I'll cone to appreciate later, but not yet. Firefox update is so fat, it forgets a tab's setting just going to a different tab -- productivity is horrible. Jerky load. Just seems to hang ........  then continues. New look is obtuse. Yeah, and add some kind of rudimentary bookmark editing and grouping. Back to trying Google and Safari again.</t>
@@ -447,58 +524,61 @@
     <t>Good Safari alterna. Possibly the best alternative to Safari on iOS. Not without it's faults though. I've never liked Top Sites, preferring to store my own sites. Although you can pin sites here, you cannot rearrange the order which is annoying. Once you navigate away from Top Sites, Bookmarks etc. there's no simple way to access these unless you open a new tab. A button on the menu bar would solve this. I also like the Safari approach that uses a drop down menu when you click on the search/address bar. I do welcome the tracker blocker but wish we could have an ad blocker too as ads eat into mobile data and take up too much room on smaller screens. Also could do with a 'do not track' request and the option to block 3rd party cookies, which I do on Firefox desktop. I would also like an easier way to delete private data as having to go through several menus before I close the browser is very tedious and irritating - it's a shame mobile devices loose the handy keyboard shortcuts desktop browsers have. Perhaps Firefox iOS could delete private data when you close the browser like the desktop browser does. I'll stick with Safari and keep Firefox to track it's progress and use for the occasional site that doesn't work properly in Safari.</t>
   </si>
   <si>
-    <t>¾Ð¡äö¾ÏÂ_üü´_Ó¬. ¾Ð¡äö¾ÏÂüÓª_Î_ÏÑ«¾¬Á__Ùà¼¤¼ _ÙÔ</t>
+    <t>新版本非常好用. 新版本不错，夜间模式也升级了👍</t>
   </si>
   <si>
     <t>Adding block ads. Need to improve the performance and the speed of browsing the web. The management of the tag in the form of a larger window and can turn left or right to manage the tag. Can top up paws the screen to close the tag. Thank developers</t>
   </si>
   <si>
-    <t>Safari âöâ_ãã. â¢ÄÄÄÑÄàÄ_ÄöÑ_Üâäâ¢â_â_Ä_Ü£Òâö»£ÙÑÛPC¤_Ü_ÙâÀÄÐâÕiPhone¤¦_âÕ_ÜâÜÒ¬ââ¤âÜÛâ</t>
+    <t>Safari よりいい. アップデートしてからアイコンかっこよくなったし、PCで見てたタブをiPhoneで続きを見ることもできる。</t>
   </si>
   <si>
     <t>Great update. The experience is much better, having access to more in the lower half of the screen was sorely needed, my thumb thanks you.</t>
   </si>
   <si>
-    <t>Au top ! _ÙÔ_ÙÈ. Bonjour aux dÌ©veloppeurs de Firefox, navigateur trÌ¬s fluide et rapide comme toujours, jÛªaime bien Firefox sur pc et sur iPhone cÛªest bien aussi. Le seul reproche que jÛªai ÌÊ faire dans cette mise ÌÊ jour, cÛªest dÛªavoir changer lÛªinterface avec cette couleur trop sombre, la couleur blanche Ì©tait beaucoup mieux, sa mettais plus en valeur le navigateur. _x000D_Bonne continuation ÌÊ vous...</t>
+    <t>Au top ! 👍🏻. Bonjour aux développeurs de Firefox, navigateur très fluide et rapide comme toujours, j’aime bien Firefox sur pc et sur iPhone c’est bien aussi. Le seul reproche que j’ai à faire dans cette mise à jour, c’est d’avoir changer l’interface avec cette couleur trop sombre, la couleur blanche était beaucoup mieux, sa mettais plus en valeur le navigateur. 
+Bonne continuation à vous...</t>
   </si>
   <si>
     <t>Choose the side of dark. Love latest update! Thnx to devs</t>
   </si>
   <si>
-    <t>Bad update. Few time address bar search opens previously closed page. Few website contents abruptly stopped loading, it views only partial page. I donÛªt know how such update rolled out with any quality check... literally it made me to stop using the Firefox.</t>
-  </si>
-  <si>
-    <t>0 _ü. LÌ_ÌÙt sich auf meinem Ipad Air Ì_berhaupt nicht Ì¦ffnen.</t>
+    <t>Bad update. Few time address bar search opens previously closed page. Few website contents abruptly stopped loading, it views only partial page. I don’t know how such update rolled out with any quality check... literally it made me to stop using the Firefox.</t>
+  </si>
+  <si>
+    <t>0 ⭐️. Läßt sich auf meinem Ipad Air überhaupt nicht öffnen.</t>
   </si>
   <si>
     <t>Schlimm Besserung. Das neue Logo sieht schei*e aus!</t>
   </si>
   <si>
-    <t>üâü_ü´ü_üà_Äü__ä_ü_üÝ üã_äüªüÇü__Äüª_Ûü¤_àü__ãüÜü¥_Î_üªü¡üªü_ü¤_öü_üÓüµ. üâü_ü´ü_üà_Äü__ä_ü_üÝ üã_äüªüÇü__Äüª_Ûü¤_àü__ãüÜü¥_Î_üªü¡üªü_ü¤_öü_üÓüµ üÐ_äü_üÓüµüöü£ü«üàüöü¡_üªü¡üªü__Ûü_üá_öü_üªü¥_öü_üã_öü¡</t>
-  </si>
-  <si>
-    <t>Love the new clean look. FirefoxÛªs latest release looks good!</t>
-  </si>
-  <si>
-    <t>A great new effort but.... This latest update to Firefox is excellent but I really donÛªt like the fact that when I type part of a website address, itÛªs often not able to complete the rest intelligently from which point  I could then tap Enter and go to the site (like Safari).  _x000D__x000D_Also, the search suggestions need reworking.  I typed cnn and, meaning to complete it with a .com, a search suggestion displayed as if IÛªd wanted to search Google for cnn.com.</t>
-  </si>
-  <si>
-    <t>_ÙÎÙ_ÙÎÙAhora si la App 1 de navegacion_ÙÎÙ _ÙÎÙ. _ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙNavegador predeterminado? No,ya es mi navegador por default,ese nuevo color le queda al 100000,grasias firefox _ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ</t>
-  </si>
-  <si>
-    <t>Please Remove the New Tab Popup!. Ever since version 6.0 or 7.0, there is an annoying blue pop up on the bottom of my screen whenever I open a new tab. It is so annoying I stopped using Firefox and went back to Chrome._x000D__x000D_Please give us an option to disable that pop up. I love the interface changes in 10.0 and I want to use them, but I canÛªt stand that pop up at all and wonÛªt use Firefox until itÛªs gone or thereÛªs an option to turn it off.</t>
+    <t>ขอลองใช้แอป ค้นหาในเว็บไซต์แนะนำว่าดี. ขอลองใช้แอป ค้นหาในเว็บไซต์แนะนำว่าดี ถ้าดีจริงจะแนะนำเพื่อนต่อค่ะ</t>
+  </si>
+  <si>
+    <t>Love the new clean look. Firefox’s latest release looks good!</t>
+  </si>
+  <si>
+    <t>A great new effort but.... This latest update to Firefox is excellent but I really don’t like the fact that when I type part of a website address, it’s often not able to complete the rest intelligently from which point  I could then tap Enter and go to the site (like Safari).  
+Also, the search suggestions need reworking.  I typed cnn and, meaning to complete it with a .com, a search suggestion displayed as if I’d wanted to search Google for cnn.com.</t>
+  </si>
+  <si>
+    <t>🌟🌟Ahora si la App 1 de navegacion🌟 🌟. 🌟🌟🌟🌟Navegador predeterminado? No,ya es mi navegador por default,ese nuevo color le queda al 100000,grasias firefox 🌟🌟🌟🌟🌟🌟</t>
+  </si>
+  <si>
+    <t>Please Remove the New Tab Popup!. Ever since version 6.0 or 7.0, there is an annoying blue pop up on the bottom of my screen whenever I open a new tab. It is so annoying I stopped using Firefox and went back to Chrome.
+Please give us an option to disable that pop up. I love the interface changes in 10.0 and I want to use them, but I can’t stand that pop up at all and won’t use Firefox until it’s gone or there’s an option to turn it off.</t>
   </si>
   <si>
     <t>Fast. Very fast</t>
   </si>
   <si>
-    <t>Geht und ist hipp. Hipper browser und schÌ¦nes erscheinungsbild. Seit dem neuen update nun auch eine funktionierende darstellung von icons</t>
-  </si>
-  <si>
-    <t>_Ù_. _÷_á___µ___µ___ü _À__Û_¡_«_____¡_È_ü, _À___ÈÎ_á_____¡âÎ _È_ü_üà_¼____ â_µ_À_µÛÎ ___¡__________ Ä_«___±___µ_µ, _µ_«_ü__â___µ_______µ, ___¡Û_ü_¡â_ü______âÎ ___ü_«_¡ ___¼_È_¡_«___¼ __Ô _¦_µ _«___È_¦___¡ _±ÜâÎ (_____±___«Ä _¼_____µÛ___¡__). __à_µ__Î É__â_µ_È__Î _±Ü _ü___µâÎ _±_È___¼_üÛ____ä_ü_¼ Û_µ_¼_È_¡__Ü ____ÄâÛ_ü _±Û_¡Ä_á_µÛ_¡, _¼__â__ÛÜ__ _ÀÛ__É___«_ü_È _±Ü â_µâ à_µ_¼_¡_«_±_È___¼, _µâÎ _À_¡Û__à_¼_¡ _±Û_¡Ä_á_µÛ____ àâ__ _ÀÛ__É___«â _µ____ ___¡_À___È_____ü__Ä, Û_¡_±__â_¡  Û_µ_¼_È_¡______ Ä ___üÉ Û_¡_á___üâ, _¡ _À___ÈÎ_á_____¡âÎ _ü___ü ___µ_ÀÛ_ü__Üà____ _ü ___µÄ_«___±____.</t>
-  </si>
-  <si>
-    <t>Melhorou!. Ainda falta melhorar a resoluÌ¤Ì£o do logo do Google ao fazer pesquisas....sÌ_ isso que me incomoda em relaÌ¤Ì£o ao Safari</t>
+    <t>Geht und ist hipp. Hipper browser und schönes erscheinungsbild. Seit dem neuen update nun auch eine funktionierende darstellung von icons</t>
+  </si>
+  <si>
+    <t>🐼. Изменения порадовали, пользоваться лисичкой теперь намного удобнее, единственное, вариативность вида вкладок всё же должна быть (свободу консервам). Очень хотелось бы иметь блокировщик рекламы внутри браузера, который проходил бы тест чекадблок, есть парочка браузеров что проходят его наполовину, работа с рекламой у них разнится, а пользоваться ими непривычно и неудобно.</t>
+  </si>
+  <si>
+    <t>Melhorou!. Ainda falta melhorar a resolução do logo do Google ao fazer pesquisas....só isso que me incomoda em relação ao Safari</t>
   </si>
   <si>
     <t>Best browser. It's the fastest browser I have. I would like to know where the setting is to not load images in the new version. I can't find it anywhere</t>
@@ -507,34 +587,53 @@
     <t>Dark icon. Thank you for not having yet another icon on a white background.</t>
   </si>
   <si>
-    <t>Bester Browser. Ich bin schon immer Firefox Fan und nutze den Browser auf dem Smartphone, sowie dem Desktop. FÌ_r die UnterstÌ_tzung der Verwaltung von Bookmarks und dass sich im Privaten Modus gescannte QR-Codes, auch in diesem Ì¦ffnen, gibt es den fÌ_nften Stern.</t>
+    <t>Bester Browser. Ich bin schon immer Firefox Fan und nutze den Browser auf dem Smartphone, sowie dem Desktop. Für die Unterstützung der Verwaltung von Bookmarks und dass sich im Privaten Modus gescannte QR-Codes, auch in diesem öffnen, gibt es den fünften Stern.</t>
   </si>
   <si>
     <t>Night mode. A great web browser with privacy in mind. One small issue: night mode simply inverses the page colors, assuming a white background. However, it also inverses the page colors when the background color is already black, which results in a bright white background.</t>
   </si>
   <si>
-    <t>_Ê_µ_¦_ü__ _ü___¼_______üâ__. _Á_«_µ_È_¡__â_µ â_¡_¼, àâ___±Ü __ Û_µ_¦_ü___µ _ü___¼_______üâ__ _ÀÛ_ü __â_¼ÛÜâ_ü_ü __________ ___¼_È_¡_«_¼_ü ___¡ ___«______ _ü â____ _¦_µ _¡__â_µ ___µ _ÀÛ___üÉ___«_ü_È_¡ _«_µ_¡__â__Û_ü_á_¡ _ü. __¡ _¼_____ÀÎ_â_µÛ______ ___µÛ_ü_ü â_¡_¼______ ___µâ.</t>
-  </si>
-  <si>
-    <t>Bester Browser. Mein liebster Browser auf allen Systemen. Kommt schick und leistungsfÌ_hig daher. Mir fehlt nur noch ein AdBlocker Add-On. Leider unterstÌ_tzt er immer noch keine selbstaufgesetzten Sync Server, wirklich schade...</t>
-  </si>
-  <si>
-    <t>Top App. Das neue Design gefÌ_llt mir echt gut_ÙÔ_ÙÈ Die App lÌ_sst sich einfach bedienen und lÌ_uft flÌ_ssig.</t>
-  </si>
-  <si>
-    <t>Schlimm.... - potthÌ_ÌÙlich, die neue UI noch schlimmer als die alte_x000D_- Lesezeichenverwaltung erbÌ_rmlich_x000D_- trÌ_ge und langsam_x000D_- selbst auf der Mozilla-Seite schon Fehldarstellungen_x000D_- ungefragte, unerwÌ_nschte und nicht abschaltbare Û_EmpfehlungenÛÏ gehen gar nicht!!_x000D__x000D_Mozilla schafft sich so langsam selber ab. Sowohl bei den Apps als auch bei den Desktopversionen. Wenn nur der Safari nicht noch schlechter wÌ_re... :(</t>
-  </si>
-  <si>
-    <t>Needs UI tweaking and Adblocking integration. Dear Mozilla,_x000D__x000D_This is a product with tons of opportunities. The custom search engine script is amazing, and finally allows me to use a custom search query for a trustworthy engine (StartPage). This finally pulls me away from the control of Google. However, some tweaks would make it a better product on iPad and iPhone:_x000D__x000D_1) Add Adblocking ability from Firefox Focus. I realize that it is no small feat as Apple does not allow Firefox iOS to use the apple scripts for Adblocking, but adopting the block lists to the fully fledged app would be a gift to all._x000D__x000D_Update: 9/22/2017. Thank you for adding tracking protection, and at different levels! This is a huge improvement for user privacy and I commend Mozilla for continuing to fight the good fight against tracking._x000D__x000D_2) Make bookmarks editable (renamable) and their order organizable. Currently you can only delete or open them in a new tab as options. It's not a mature feature set._x000D__x000D_3) Move the new tab button on the tab viewing page from the bottom left to the bottom right. This keeps you from having to travel the diagonal from the tab button (upper right) to the opposite (bottom left) corner, switching hands. Useful on iPad, VERY USEFUL for iPhone use, which is often one handed._x000D__x000D_Update 11/9/2017_x000D_The good guys at Mozilla DID IT! The new ÛÏphotonÛ layout is easier than ever to use! Thanks for listening to users and making the UI more accessible!_x000D__x000D_4) the pin to top sites feature only allows one link to the domain of choice. If I want to have a link to my Amazon Orders, that will take over the general Amazon.com link. Make this more like the safari Favorites tab! There's no need to reinvent the wheel. Customization, privacy, and autonomy should be the hallmark of Firefox. Not some gimmicky, clunky suggested websites. What if I visit an illicit website and don't want to worry about it poppin up in a new tab?? I get it, use private browsing mode, but the suggested websites panel should be an option you can disable._x000D__x000D_Lots of potential, but the app needs some streamlining and more options for the user. Apple locks us down, but Mozilla can potentially set us free.</t>
-  </si>
-  <si>
-    <t>Super Browser. Benutze seit Jahren Firefox am PC, auch auf iOS kann ich ihn nur weiterempfehlen. Nebenbei ist es fÌ_r einen guten Zweck, da Mozilla jeden das Internet zugÌ_nglich machen will.</t>
+    <t>Режим инкогнито. Сделайте так, чтобы в режиме инкогнито при открытии новой вкладки на одном и том же сайте не происходила деавторизация. На компьютерной версии такого нет.</t>
+  </si>
+  <si>
+    <t>Bester Browser. Mein liebster Browser auf allen Systemen. Kommt schick und leistungsfähig daher. Mir fehlt nur noch ein AdBlocker Add-On. Leider unterstützt er immer noch keine selbstaufgesetzten Sync Server, wirklich schade...</t>
+  </si>
+  <si>
+    <t>Top App. Das neue Design gefällt mir echt gut👍🏻 Die App lässt sich einfach bedienen und läuft flüssig.</t>
+  </si>
+  <si>
+    <t>Schlimm.... - potthäßlich, die neue UI noch schlimmer als die alte
+- Lesezeichenverwaltung erbärmlich
+- träge und langsam
+- selbst auf der Mozilla-Seite schon Fehldarstellungen
+- ungefragte, unerwünschte und nicht abschaltbare „Empfehlungen“ gehen gar nicht!!
+Mozilla schafft sich so langsam selber ab. Sowohl bei den Apps als auch bei den Desktopversionen. Wenn nur der Safari nicht noch schlechter wäre... :(</t>
+  </si>
+  <si>
+    <t>Needs UI tweaking and Adblocking integration. Dear Mozilla,
+This is a product with tons of opportunities. The custom search engine script is amazing, and finally allows me to use a custom search query for a trustworthy engine (StartPage). This finally pulls me away from the control of Google. However, some tweaks would make it a better product on iPad and iPhone:
+1) Add Adblocking ability from Firefox Focus. I realize that it is no small feat as Apple does not allow Firefox iOS to use the apple scripts for Adblocking, but adopting the block lists to the fully fledged app would be a gift to all.
+Update: 9/22/2017. Thank you for adding tracking protection, and at different levels! This is a huge improvement for user privacy and I commend Mozilla for continuing to fight the good fight against tracking.
+2) Make bookmarks editable (renamable) and their order organizable. Currently you can only delete or open them in a new tab as options. It's not a mature feature set.
+3) Move the new tab button on the tab viewing page from the bottom left to the bottom right. This keeps you from having to travel the diagonal from the tab button (upper right) to the opposite (bottom left) corner, switching hands. Useful on iPad, VERY USEFUL for iPhone use, which is often one handed.
+Update 11/9/2017
+The good guys at Mozilla DID IT! The new “photon” layout is easier than ever to use! Thanks for listening to users and making the UI more accessible!
+4) the pin to top sites feature only allows one link to the domain of choice. If I want to have a link to my Amazon Orders, that will take over the general Amazon.com link. Make this more like the safari Favorites tab! There's no need to reinvent the wheel. Customization, privacy, and autonomy should be the hallmark of Firefox. Not some gimmicky, clunky suggested websites. What if I visit an illicit website and don't want to worry about it poppin up in a new tab?? I get it, use private browsing mode, but the suggested websites panel should be an option you can disable.
+Lots of potential, but the app needs some streamlining and more options for the user. Apple locks us down, but Mozilla can potentially set us free.</t>
+  </si>
+  <si>
+    <t>Super Browser. Benutze seit Jahren Firefox am PC, auch auf iOS kann ich ihn nur weiterempfehlen. Nebenbei ist es für einen guten Zweck, da Mozilla jeden das Internet zugänglich machen will.</t>
   </si>
   <si>
     <t>It's wonderful. I love the new Photon look!</t>
   </si>
   <si>
-    <t>Switched from Chrome. Really like Firefox and the new version 10 Photon look. Good job! I found it way faster than Chrome. Firefox definitely has users in mind. It offers to block ads and trackers, along with other great features, such as the long-press navigation history, and the new Night Mode and Hide Images buttons._x000D__x000D_Two new features I'd love to see are: _x000D_1) A search/filter box in the Open Tabs (ExposÌ©) interface;_x000D_2) Swiping on the URL/Menu bar lets you quickly switch to adjacent tabs, like in Chrome._x000D__x000D_Can we have them please? _Ùª_x000D__x000D_BTW, the two flyout/dropdown menus in version 10 on iPad have this translucent effect. It can be quite hard to see the menu texts depending on the web page underneath. Please make them less translucent.</t>
+    <t>Switched from Chrome. Really like Firefox and the new version 10 Photon look. Good job! I found it way faster than Chrome. Firefox definitely has users in mind. It offers to block ads and trackers, along with other great features, such as the long-press navigation history, and the new Night Mode and Hide Images buttons.
+Two new features I'd love to see are: 
+1) A search/filter box in the Open Tabs (Exposé) interface;
+2) Swiping on the URL/Menu bar lets you quickly switch to adjacent tabs, like in Chrome.
+Can we have them please? 🙏
+BTW, the two flyout/dropdown menus in version 10 on iPad have this translucent effect. It can be quite hard to see the menu texts depending on the web page underneath. Please make them less translucent.</t>
   </si>
   <si>
     <t>iPhone 7 plus. Adblock please!</t>
@@ -543,40 +642,41 @@
     <t>Looks good but I think I lost some tabs. The app looks nice but when I updated it seems that I lost some opened tabs?</t>
   </si>
   <si>
-    <t>Nova versÌ£o melhorou bastante. Esse programa Ì© apenas uma interface grÌÁfica/skin para o Safari pois a Apple nÌ£o permite o uso dos motores de terceiros no iOS(Gecko, WebKit, Blink) . De qualquer forma essa Ì© a melhor "skin" para o Safari que eu encontrei. A Mozilla estÌÁ de parabÌ©ns, dez a zero no Skin do Chrome.</t>
-  </si>
-  <si>
-    <t>__â_È_üà_____µ ___±_______È_µ___ü_µ!. _Ù___È_µ ___±_______È_µ___ü _¼_____À_¼_¡ Ä_ÀÛ_¡___È_µ___ü ___¼_È_¡_«_¼_¡___ü ___¡_¼_____µ -â__ _À___È_á_È_¡ _____ü_á, ___«_µ _µ__ ______Äâ _À___ÈÎ_á_____¡âÎ _È__«_ü  _¼__Û__â_¼_ü___ü _À_¡_ÈÎ _¡___ü, _ü â_µ_À_µÛÎ _±Û_¡Ä_á_µÛ _ÀÛ__â__ _±_______À___«___±_µ__))</t>
+    <t>Nova versão melhorou bastante. Esse programa é apenas uma interface gráfica/skin para o Safari pois a Apple não permite o uso dos motores de terceiros no iOS(Gecko, WebKit, Blink) . De qualquer forma essa é a melhor "skin" para o Safari que eu encontrei. A Mozilla está de parabéns, dez a zero no Skin do Chrome.</t>
+  </si>
+  <si>
+    <t>Отличное обновление!. После обновления кнопка управления вкладками наконец-то сползла вниз, где ей могут пользоваться люди с короткими пальцами, и теперь браузер просто богоподобен))</t>
   </si>
   <si>
     <t>Upgrade removes HOME button from front!!!. Why????</t>
   </si>
   <si>
-    <t>Switched from Chrome. Really like Firefox and the new version 10 Photon look. Good job! I found it way faster than Chrome. Firefox definitely has users in mind. Love it can block ads and trackers, along with other great features, such as the long-press navigation history, and the new Night Mode and Hide Images buttons._x000D__x000D_One new feature I'd love to see is a search/filter box in the Open Tabs (ExposÌ©) interface. Can we have it please? _Ùª</t>
-  </si>
-  <si>
-    <t>iOS11.0.3¤_áö¦µâ¼ ÄÇÄ_ÄÑ. PCäöø¨ä¨_Ñ__â_Ûà¨Ñ_ãâÜ¨ÇÛiOS11.0.3¤µáÜ¥_ÎªÇ_áö¦µâ¼ âÕ_¡â_ÀÓÑ_Û_Àãä©Ç»âä»ãÛâÜ¥_Ï¾_Ï¬_Ñ_Û¨ä¨_äöâÕÉÂÐÜÑ_¾Â_Ñã_</t>
+    <t>Switched from Chrome. Really like Firefox and the new version 10 Photon look. Good job! I found it way faster than Chrome. Firefox definitely has users in mind. Love it can block ads and trackers, along with other great features, such as the long-press navigation history, and the new Night Mode and Hide Images buttons.
+One new feature I'd love to see is a search/filter box in the Open Tabs (Exposé) interface. Can we have it please? 🙏</t>
+  </si>
+  <si>
+    <t>iOS11.0.3で強制終了ループ. PC版は安定しており、重宝しているのに、iOS11.0.3で起動後すぐに強制終了を繰り返して、使い物にならない。動作検証して、安定版を公開して欲しい！</t>
   </si>
   <si>
     <t>No WebRTC :(. Firefox please add WebRTC support :(</t>
   </si>
   <si>
-    <t xml:space="preserve">Àªü»Ý_¾Êà_»ü_Ê¾Äø¼ . Àªü»Ý_¾Êà_ã¼¥ä_¾÷øÈÔä__ã_Î_»ü_Ê¾Äø¼ </t>
-  </si>
-  <si>
-    <t>Excelente. AtualizaÌ¤Ì£o ficou muito top, levinho</t>
-  </si>
-  <si>
-    <t>Ä¥Ä»ÄÄâø¨ÀÏ. Û_âÛÛ¾öÈâÜ¨ÄÐÄ»ÄÄâø¾Ò_ÏÎÇøÜâä_¤¾ÎàâÕÜ¥Ü¥»ã¬ãÔ»Ûâ_ÄöÄÂâ_âÕ¾ãÙ÷âÜÛâ__¨¤ø»Û¾Ò_Ï¤ÀÏªâÜâö Ç_äö_¾Â_ÑãÛâ</t>
-  </si>
-  <si>
-    <t>Seems more like 1.0. So weÛªre up to version 10 and you still canÛªt rename, reorder, organize, or edit bookmarks?</t>
-  </si>
-  <si>
-    <t>Excelente. Me encanta el proyecto Firefox! Esta actualizaciÌ_n estÌÁ perfecta para mÌ_ gustos! Combina todo lo bueno! Y lo mÌÁs importante es que es mÌÁs segura y mÌÁs privada! _ÙÔ</t>
-  </si>
-  <si>
-    <t>Version 10 is the Best Yet!. Everything I could ask for in a mobile browser. Great work Firefox mobile team _ÙÔ</t>
+    <t>这个图标太不习惯了. 这个图标的底色是黑色的，太不习惯了</t>
+  </si>
+  <si>
+    <t>Excelente. Atualização ficou muito top, levinho</t>
+  </si>
+  <si>
+    <t>フリックの反応. 進む、戻るのブリック操作が端から大きく指を動かさないといけなく、ストレスを感じる。位置ではなく、操作で反応するように変えて欲しい。</t>
+  </si>
+  <si>
+    <t>Seems more like 1.0. So we’re up to version 10 and you still can’t rename, reorder, organize, or edit bookmarks?</t>
+  </si>
+  <si>
+    <t>Excelente. Me encanta el proyecto Firefox! Esta actualización está perfecta para mí gustos! Combina todo lo bueno! Y lo más importante es que es más segura y más privada! 👍</t>
+  </si>
+  <si>
+    <t>Version 10 is the Best Yet!. Everything I could ask for in a mobile browser. Great work Firefox mobile team 👍</t>
   </si>
   <si>
     <t>Almost my daily browser. I would use this browser as my primary if the night mode was actually.., well night mode. The ui is still white. The idea of night mode is to use dark colours to ease your eyes. For now I'll be keeping chrome as my primary</t>
@@ -585,70 +685,83 @@
     <t>A big improvement. I've always been a Firefox fan and was happy when it finally came out on iOS. The early versions were pretty basic. I'm quite impressed with the November update.  Night mode is great and the tabs have been improved. I think I will definitely use this as an alternative to Chrome and Safari.  Good job Mozilla!</t>
   </si>
   <si>
-    <t>Perfecta. Es la app de mas uso que tengo, es simplemente  perfecta y el nuevo estilo que le dieron es hermoso. Muy buen trabajo los felicito, sigan asÌ_.</t>
-  </si>
-  <si>
-    <t>______¡ _ü_¼_____¼_¡. _Á_«_µ_È_¡__â_µ ã____ _ü_¼_____¼_ü ___µâ_È_µ_µ.</t>
-  </si>
-  <si>
-    <t>Much better UI. The new UI update is finally what firefox has needed for ios. Also the tracking protection option for ÛÏalways onÛ is a big bonus.</t>
-  </si>
-  <si>
-    <t>muito veloz. Essa nova atualizaÌ¤Ì£o estÌÁ rÌÁpida que nem uma bala ParabÌ©ns _ÙÔ_ÙÔ_ÙÔ Mozilla_x000D_SÌ_ falta colocar um tema preto no App.</t>
-  </si>
-  <si>
-    <t>You removed the only interesting feature.... Hi,_x000D_You removed in your new version the only feature that saved us some time when opening a new tab on a blank page._x000D_We didn't have to click on the search area to type a research and now we need to._x000D_Correct this ASAP._x000D_I still don't understand why I'm doing your job instead of you. #contactme #rewardnecessary _x000D_You're welcome anyway</t>
-  </si>
-  <si>
-    <t>Review. Sync tabs but no sync for logins._x000D_Used to previous/old UI, not sure if I'll like the new one._x000D_Feels faster, that's good</t>
-  </si>
-  <si>
-    <t>±Éã¦ü±Ó__ÀÔ_. ±Éã¦ü±Ó__ÀÔ__x000D_±Éã¦ü±Ó__ÀÔ__x000D_±Éã¦ü±Ó__ÀÔ_</t>
-  </si>
-  <si>
-    <t>_Ý__±_ü__Ü__ _±Û_¡Ä_á_µÛ. __â_«_µ_ÈÎ_____µ _À_¡_ü_±__ _á_¡ ãÄ___¼ _ü_ _À_µÛ_µ_«_¡à_ü ___¼_È_¡_«_¼_ü ___¡ _«ÛÄ___ü_µ ÄâÛ____â___¡!</t>
+    <t>Perfecta. Es la app de mas uso que tengo, es simplemente  perfecta y el nuevo estilo que le dieron es hermoso. Muy buen trabajo los felicito, sigan así.</t>
+  </si>
+  <si>
+    <t>Новая иконка. Сделайте фон иконки светлее.</t>
+  </si>
+  <si>
+    <t>Much better UI. The new UI update is finally what firefox has needed for ios. Also the tracking protection option for “always on” is a big bonus.</t>
+  </si>
+  <si>
+    <t>muito veloz. Essa nova atualização está rápida que nem uma bala Parabéns 👏👏👏 Mozilla
+Só falta colocar um tema preto no App.</t>
+  </si>
+  <si>
+    <t>You removed the only interesting feature.... Hi,
+You removed in your new version the only feature that saved us some time when opening a new tab on a blank page.
+We didn't have to click on the search area to type a research and now we need to.
+Correct this ASAP.
+I still don't understand why I'm doing your job instead of you. #contactme #rewardnecessary 
+You're welcome anyway</t>
+  </si>
+  <si>
+    <t>Review. Sync tabs but no sync for logins.
+Used to previous/old UI, not sure if I'll like the new one.
+Feels faster, that's good</t>
+  </si>
+  <si>
+    <t>居然不屏蔽广告. 居然不屏蔽广告
+居然不屏蔽广告
+居然不屏蔽广告</t>
+  </si>
+  <si>
+    <t>Любимый браузер. Отдельное спасибо за функцию передачи вкладки на другие устройства!</t>
   </si>
   <si>
     <t>toller browser, danke mozilla. gefaellt mir was ihr macht. tolles neues design. danke fuer blocking, nicht tracking etc.</t>
   </si>
   <si>
-    <t>Î¾_´ÓµãÔÇø____¾ÏäÑ¨¢÷_Îü¾÷ø¾ÏÛ¾Ð¡_ãÛâ. øáÀ¨_</t>
-  </si>
-  <si>
-    <t>ÀÈ¬_¾©ÙÄ_Î¾Â_Ñã. â_Ä_âÀÄ¥â¤Ä_â_Î¾Ó_Ðã¥âÎ_Û_üüÇ_Àãâãª»â__ÑÙÛâ_x000D_â¬ÛÀÈ¬_¾©ÙÄ__Ùøâ¢Ääâ»Ä_¾©ÙÄ_âÕÀ__ÊÑ_âÎÙâäÛüàÄ_ÄÐÄ©â_â¦Ç»â__ªÛâ</t>
-  </si>
-  <si>
-    <t>ÓµãÔÎ¾_´¾Ý«¾Ð¡57äö¾ÏÂ¼ _ÎÒö. ¾Ð¡äö¾ÏÂ_Î¾Ð¡¥Î¢_ÎÐÏ¾Â¢</t>
-  </si>
-  <si>
-    <t>Version 10. Das neue Design ist sehr gelungen und die Anordnung der SchaltflÌ_chen sinnvoll. _x000D__x000D_Jetzt fehlt mir nur noch die MÌ¦glichkeit Lesezeichen sortieren und in Ordner packen zu kÌ¦nnen. Wie im Safari Browser eben. _x000D__x000D_Soweit aber wirklich gelungen.</t>
-  </si>
-  <si>
-    <t>_£_¦_¡____!. _Á___µ___üâ_µ ã____ Ä _ü_¼_____¼_ü: Ä_±_µÛ_üâ_µ à_µÛ__Ü__!!! _÷ _«_µ_È_¡__â_µ _ÀÛ_µ_«_È___¦_µ___ü _À___ü_¼____ÜÉ _üâ_µ__ __â_¼_È_à_¡_µ__Ü___ü: â__Û_____á_üâ Ä_¦_¡____!!!</t>
+    <t>同步电脑端书签有问题，不是最新的。. 请修复</t>
+  </si>
+  <si>
+    <t>翻訳機能が欲しい. インタフェースが改善されて、非常に使いやすくなりました。
+あと、翻訳機能またはアドオン機能を追加してくれたら、万能ブラウザになります。</t>
+  </si>
+  <si>
+    <t>电脑同步更新57版本了，哈. 新版本，新界面，喜欢</t>
+  </si>
+  <si>
+    <t>Version 10. Das neue Design ist sehr gelungen und die Anordnung der Schaltflächen sinnvoll. 
+Jetzt fehlt mir nur noch die Möglichkeit Lesezeichen sortieren und in Ordner packen zu können. Wie im Safari Browser eben. 
+Soweit aber wirklich gelungen.</t>
+  </si>
+  <si>
+    <t>Ужасно!. Смените фон у иконки: уберите черный!!! И сделайте предложения поисковых систем отключаемыми: тормозит ужасно!!!</t>
   </si>
   <si>
     <t>bookmark. bookmark couldn't be reordered</t>
   </si>
   <si>
-    <t>SÌ_peerr. Kulland±Ù±m en iyi taray±c± _ÙÔ</t>
-  </si>
-  <si>
-    <t>É_¼__ÏÑ«¾¬Á_. üÎ¾ÏÝÏ¬_Û_ÏÑ«¾¬Á___Î____ÕÎ_ _¨¡_¥_ÙÄ_¾÷ø_ÏÑ«üÈ¢÷_ÎÉ¦ÈÐÀ÷´__Î¾Óø¾ÎüÛüÜ</t>
-  </si>
-  <si>
-    <t>__µ _á_¡ö_È__. ___¡_¼-â__ ___µ _á_¡ö_È__ ___±_______È_µ___ü_µ. ___¡_¼___µ â__ ___ÈÄ_À___µ _À___«Û_¡_¦_¡___ü_µ Chrome. _Ó__ â______ Ä ___¡ _±Ü_È _ü___«_ü___ü_«Ä_¡_ÈÎ__Ü__ â_ü_ÈÎ, _¼__â__ÛÜ__ __â_È_üà_¡_È ___¡ __â _«ÛÄ___üÉ _±Û_¡Ä_á_µÛ____. _Á_µ__à_¡ â_ü __Û_¡___ü Ü âÔÛâÜ, àÔÛ__Ü_µ _ü_¼_____¼_ü __Ü___È_«â Ä_±______, _____µ__ ___µ __ â_ü_È_µ Firefox.</t>
-  </si>
-  <si>
-    <t>Better than Chrome. Not only is it better than Chrome, itÛªs better than every other browser there is. Firefox is now in the lead for security, speed, and support with their ÛÏquantumÛ project.</t>
-  </si>
-  <si>
-    <t>Î¾_´üÄ_Ó¬. ¾ÊÁ»Îâ¨¨±üÄ_Ó¬</t>
-  </si>
-  <si>
-    <t>Depois da atualizaÌ¤Ì£o ficou melhor ainda. O melhor navegador, com design lindo e intuitivo, uso tambÌ©m no desktop. Meu principal navegador ªÁ</t>
-  </si>
-  <si>
-    <t>Wow!. This update is amazing!  Love the new look and feel.  ItÛªs like a whole new app!</t>
+    <t>Süpeerr. Kullandığım en iyi tarayıcı 👍</t>
+  </si>
+  <si>
+    <t>关于夜间模式. 希望在开夜间模式后，书签和历史记录也能是夜间主题，其他还好，支持一下</t>
+  </si>
+  <si>
+    <t>Не зашло. Как-то не зашло обновление. Какое то глупое подражание Chrome. До этого у вас был индивидуальный стиль, который отличал вас от других браузеров. Сейчас эти границы стёрты, чёрные иконки выглядят убого, совсем не в стиле Firefox.</t>
+  </si>
+  <si>
+    <t>Better than Chrome. Not only is it better than Chrome, it’s better than every other browser there is. Firefox is now in the lead for security, speed, and support with their “quantum” project.</t>
+  </si>
+  <si>
+    <t>同步不能用. 校验邮箱不能用</t>
+  </si>
+  <si>
+    <t>Depois da atualização ficou melhor ainda. O melhor navegador, com design lindo e intuitivo, uso também no desktop. Meu principal navegador ♡</t>
+  </si>
+  <si>
+    <t>Wow!. This update is amazing!  Love the new look and feel.  It’s like a whole new app!</t>
   </si>
   <si>
     <t>Excellent browser. Very Fast from my first assessment, elegant and ergonomic, and has your privacy's interest in mind - authentically. Version 57 on the desktop, with its new engine, and efficient resource footprint has now replaced Chrome.</t>
@@ -657,7 +770,8 @@
     <t>Great alternative at safari. I really like the new interface. I use this now for 90% of my webbrowsing on iPhone. Keep up the good work Firefox team!</t>
   </si>
   <si>
-    <t>Surpreendente _ÙÕ»_ÙÈ. Vale a pena o download do Firefox no iOS, roda muito fluido no meu 6s com iOS 11.1_x000D_Muito melhor que o Chrome no mobile, bom concorrente do Safari, jÌÁ no Mac OSX o Chrome dispara na frente, e o Safari e Mozilla logo atrÌÁs.</t>
+    <t>Surpreendente 💪🏻. Vale a pena o download do Firefox no iOS, roda muito fluido no meu 6s com iOS 11.1
+Muito melhor que o Chrome no mobile, bom concorrente do Safari, já no Mac OSX o Chrome dispara na frente, e o Safari e Mozilla logo atrás.</t>
   </si>
   <si>
     <t>Muito bonito... Nosso fivou bem kegal r bonito...</t>
@@ -666,10 +780,10 @@
     <t>Almost there.... The one feature I person still would love to have added is the ability to have Firefox launch into private mode and STAY in private mode (like an option to set it that way) so I don't have to switch after the fact or use 3D Touch to launch it that way. I don't want to have to set the option of not closing Private Tabs upon exit because, to me, that partially defeats the point of even using Private Tabs. They're supposed to leave no traces. The desktop version has this feature, iOS Safari has this feature, so why don't you guys do the same?</t>
   </si>
   <si>
-    <t>ZwangsbeglÌ_ckung mit Pocket ist Ì_rgerlich. Wie lÌ_sst sich das abstellen?</t>
-  </si>
-  <si>
-    <t>dark mode is cool but add smart invert please. Smart invert_Ù÷</t>
+    <t>Zwangsbeglückung mit Pocket ist ärgerlich. Wie lässt sich das abstellen?</t>
+  </si>
+  <si>
+    <t>dark mode is cool but add smart invert please. Smart invert😁</t>
   </si>
   <si>
     <t>Excellent on my Mac piece of crap on my iPad. Just copy-paste Mercury web browser. Where this extraordinary browser disappeared. FF for iOS is unstable, annoying and unreliable - don't bother to download.</t>
@@ -678,58 +792,71 @@
     <t>BETTER TABS AND 1PASSWORD SUPPORT. Wow, you guys rock! This new update fixed the two things keeping me from using Firefox: the tab button and integrated 1Password support. Both now work and I love Firefox so much!</t>
   </si>
   <si>
-    <t>FireFox is finally becoming great on iOS!!!. Firefox for iOS is finally becoming good and fast while syncing is active._x000D__x000D_Love the image block ability to limit data usage._x000D__x000D_Night mode for websites is nice but id also like the interface to be completely black.</t>
-  </si>
-  <si>
-    <t>Little hope left.. I want to use Firefox. _x000D_But it keeps pushing me away. _x000D__x000D_Why donÛªt the support password managers like the brave browser does for instance._x000D_ItÛªs only a secondary browser at best in its current form.</t>
-  </si>
-  <si>
-    <t>Tab Ansicht. Endlich ist der Schalter fÌ_r die Tabansicht unten. Endlich schneller navigieren!!!</t>
-  </si>
-  <si>
-    <t>Navegador obligatorio. Con la Ì¼ltima actualizaciÌ_n lo habÌ©is bordado !!!! Enhorabuena !!!!</t>
-  </si>
-  <si>
-    <t>Ottima. Decisamente migliore di Safari o chrome, sarebbe grandiosa la presenza dei plugin, stampa con cloud print ed un adblock integrato, ma giÌÊ cosÌÂ secondo me Ì¬ il miglior browser per ios</t>
-  </si>
-  <si>
-    <t>Finally!. Photon is here and the speed and usability is better than ever! The sync with desktop works perfectly which helps me a lot. _x000D__x000D_Sending tabs form desktop to mobile could be a little faster but overall very happy!</t>
-  </si>
-  <si>
-    <t>YEN¡ GÌÏNCELLEME SÌÏPER!. KE_KE EKLENT¡LER¡DE KULLANAB¡LSEK EEEYY FIREFOX!!</t>
-  </si>
-  <si>
-    <t>Not bad but needs more usability improvements. Finally some long awaited improvements. Still more needed._x000D__x000D_Missing a dark mode. Night mode is not quite what i expect. Twitter night mode is much better._x000D__x000D_The lower toolbar should disappear when not needed to preserve screen real estate._x000D__x000D_No option to place shortcuts on home screen?</t>
-  </si>
-  <si>
-    <t>Nice. Why the hell canÛªt we reorganised opened tabs ??? Please !!!_x000D_Another things, navigate in your favs, open a link, go back. Huh, back to root of favs !!???!!</t>
+    <t>FireFox is finally becoming great on iOS!!!. Firefox for iOS is finally becoming good and fast while syncing is active.
+Love the image block ability to limit data usage.
+Night mode for websites is nice but id also like the interface to be completely black.</t>
+  </si>
+  <si>
+    <t>Little hope left.. I want to use Firefox. 
+But it keeps pushing me away. 
+Why don’t the support password managers like the brave browser does for instance.
+It’s only a secondary browser at best in its current form.</t>
+  </si>
+  <si>
+    <t>Tab Ansicht. Endlich ist der Schalter für die Tabansicht unten. Endlich schneller navigieren!!!</t>
+  </si>
+  <si>
+    <t>Navegador obligatorio. Con la última actualización lo habéis bordado !!!! Enhorabuena !!!!</t>
+  </si>
+  <si>
+    <t>Ottima. Decisamente migliore di Safari o chrome, sarebbe grandiosa la presenza dei plugin, stampa con cloud print ed un adblock integrato, ma già così secondo me è il miglior browser per ios</t>
+  </si>
+  <si>
+    <t>Finally!. Photon is here and the speed and usability is better than ever! The sync with desktop works perfectly which helps me a lot. 
+Sending tabs form desktop to mobile could be a little faster but overall very happy!</t>
+  </si>
+  <si>
+    <t>YENİ GÜNCELLEME SÜPER!. KEŞKE EKLENTİLERİDE KULLANABİLSEK EEEYY FIREFOX!!</t>
+  </si>
+  <si>
+    <t>Not bad but needs more usability improvements. Finally some long awaited improvements. Still more needed.
+Missing a dark mode. Night mode is not quite what i expect. Twitter night mode is much better.
+The lower toolbar should disappear when not needed to preserve screen real estate.
+No option to place shortcuts on home screen?</t>
+  </si>
+  <si>
+    <t>Nice. Why the hell can’t we reorganised opened tabs ??? Please !!!
+Another things, navigate in your favs, open a link, go back. Huh, back to root of favs !!???!!</t>
   </si>
   <si>
     <t>Excellent. Great v10</t>
   </si>
   <si>
-    <t>Neue Version.... ...ist super. Grade der einfache Wechsel zur Desktop Webseite ist gold wert. Liebes Entwicklerteam ich will mich hierfÌ_r vom ganzen Herzen bedanken!</t>
-  </si>
-  <si>
-    <t>Great New Look. This is a fantastic new look. I prefer this browsers to the Google Web Browers. ItÛªs dependable and doesnÛªt crush</t>
-  </si>
-  <si>
-    <t>67 language but no Arabic !. 67 language supported , but Arabic is not included!!!!!!!!_x000D_I canÛªt understand that_x000D_This so weird and odd.</t>
+    <t>Neue Version.... ...ist super. Grade der einfache Wechsel zur Desktop Webseite ist gold wert. Liebes Entwicklerteam ich will mich hierfür vom ganzen Herzen bedanken!</t>
+  </si>
+  <si>
+    <t>Great New Look. This is a fantastic new look. I prefer this browsers to the Google Web Browers. It’s dependable and doesn’t crush</t>
+  </si>
+  <si>
+    <t>67 language but no Arabic !. 67 language supported , but Arabic is not included!!!!!!!!
+I can’t understand that
+This so weird and odd.</t>
   </si>
   <si>
     <t>Nice, but there is always more. Nice update. Now, can you do it so webpages, like YouTube or other sites that have an app version. Can you keep them from redirecting me to the installed app? I want things to stay in the browser.</t>
   </si>
   <si>
-    <t>Firefox Quantum (10.0). Sehr schÌ¦ne, schlicht und Ì_bersichtliche OberflÌ_che. Bis jetzt keine AbstÌ_rze und lÌ_uft sehr schnell. Weiter so!</t>
+    <t>Firefox Quantum (10.0). Sehr schöne, schlicht und übersichtliche Oberfläche. Bis jetzt keine Abstürze und läuft sehr schnell. Weiter so!</t>
   </si>
   <si>
     <t>Ok. Please improve the reader view. And integrate an Adblocker</t>
   </si>
   <si>
-    <t>Ottimo browser!. Adesso con Photon ha una marcia in piÌ_! Bellissimo! Bravi!_x000D_Attendo con ansia la versione desktop la prossima settimana :) W Mozilla!</t>
-  </si>
-  <si>
-    <t>Highly recommended. Works great goed_Ù_ä</t>
+    <t>Ottimo browser!. Adesso con Photon ha una marcia in più! Bellissimo! Bravi!
+Attendo con ansia la versione desktop la prossima settimana :) W Mozilla!</t>
+  </si>
+  <si>
+    <t>Highly recommended. Works great goed🎉</t>
   </si>
   <si>
     <t>Last update almost perfect!. Finally !!! Finally Firefox is almost as fluid as Safari! I really like the Mozilla philosophy but lately I had more and more trouble using their browser for Safari ... And with this update, we finally have something fluid, fast without lags ! We can finally have the list of open tabs on the bottom bar and no longer at the top (difficult to access on a Plus model). I really like the new photon interface. In short, a success. The only small point I have to blame is that to open a tab we have to go to the list of tabs and press &amp;quot;+&amp;quot;, it was a little faster on the old version with the quick menu in the middle of the bottom interface bar.</t>
@@ -744,7 +871,7 @@
     <t>Norms. normally so, does not brake, it opens quickly.</t>
   </si>
   <si>
-    <t>Icon. Too cute this new icon fox _Ù___ÙÕ¥ I love!</t>
+    <t>Icon. Too cute this new icon fox 🦊💕 I love!</t>
   </si>
   <si>
     <t>Finally, everything is fine. Version 10.1. Good update.</t>
@@ -777,7 +904,7 @@
     <t>Additional components. Hope can use additional components</t>
   </si>
   <si>
-    <t>Pitch perfect. Clearly the best browser on iOS. Integration of several search engines, speed, private browsing, complete and efficient parameters. No complaints. _ÙÔ_ÙÈ_ÙÔ_ÙÈ_ÙÔ_ÙÈ</t>
+    <t>Pitch perfect. Clearly the best browser on iOS. Integration of several search engines, speed, private browsing, complete and efficient parameters. No complaints. 👏🏻👏🏻👏🏻</t>
   </si>
   <si>
     <t>Bad Design. Dark strip at the top. It is not possible to drag and drop tabs. No banner blocker.</t>
@@ -786,7 +913,7 @@
     <t>Missing bookmark bar display!. Access to bookmarks is slow: if there was a chance to display the bookmark bar as in the desktop version ... fifth star!</t>
   </si>
   <si>
-    <t>Best. For me it is the best internet browsing apps, your ads are the most and a great help ... thanks Mozilla Group ... _ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ</t>
+    <t>Best. For me it is the best internet browsing apps, your ads are the most and a great help ... thanks Mozilla Group ... 🌟🌟🌟🌟🌟</t>
   </si>
   <si>
     <t>The browser is not secure!. Attention, when you hit a certain page, the browser allows you to open a page with certain forms that require clicking OK, if such page is opened, then no more actions in the browser can be made, the application does not allow you to close the page that caused this form. Actually, you can not do anything anymore. Only close the browser completely. It&amp;#39;s just a hole!</t>
@@ -870,16 +997,16 @@
     <t>Excellent. I already liked it and now with the new version that brings the controls on the bottom of the browser was great, much more practical. It is very light it is also with a great look.</t>
   </si>
   <si>
-    <t>The new version is very easy to use. The new version is good, night mode is also upgraded _ÙÔ</t>
+    <t>The new version is very easy to use. The new version is good, night mode is also upgraded 👍</t>
   </si>
   <si>
     <t>Better than Safari. I updated the icon and it got cool and I could see the tab I saw on the PC with my iPhone.</t>
   </si>
   <si>
-    <t>In the top ! _ÙÔ_Ù_. Hello to the developers of Firefox, browser very fluid and fast as always, I like Firefox on PC and iPhone is good too. The only complaint I have to make in this update is to change the interface with this color too dark, the white color was much better, it was more worth the browser. All the best...</t>
-  </si>
-  <si>
-    <t>0 _ü. Can not open at all on my Ipad Air.</t>
+    <t>In the top ! 👍🏼. Hello to the developers of Firefox, browser very fluid and fast as always, I like Firefox on PC and iPhone is good too. The only complaint I have to make in this update is to change the interface with this color too dark, the white color was much better, it was more worth the browser. All the best...</t>
+  </si>
+  <si>
+    <t>0 ⭐️. Can not open at all on my Ipad Air.</t>
   </si>
   <si>
     <t>Bad improvement. The new logo looks like shit!</t>
@@ -888,13 +1015,13 @@
     <t>Try using the search app on the site to suggest that it&amp;#39;s good.. Try using the search app on the site to suggest that it&amp;#39;s good. If it&amp;#39;s good, I&amp;#39;ll introduce you to me.</t>
   </si>
   <si>
-    <t>_ÙÎÙ_ÙÎÙNow if the Navigation App 1 _ÙÎÙ. _ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ Default browser? No, it&amp;#39;s already my browser by default, that new color is at 100000, firefox grasias _ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ_ÙÎÙ</t>
+    <t>🌟🌟Now if the Navigation App 1 🌟. 🌟🌟🌟🌟 Default browser? No, it&amp;#39;s already my browser by default, that new color is at 100000, firefox grasias 🌟🌟🌟🌟🌟🌟</t>
   </si>
   <si>
     <t>Goes and is hip. Hipper browser and nice appearance. Since the new update now also a working representation of icons</t>
   </si>
   <si>
-    <t>_Ù÷©. Changes pleased, using the chanterelle is now much more convenient, the only thing, the variability of the type of tabs should still be (freedom is conservative). I would very much like to have an ad blocker inside the browser that would pass the check of the checkbox, there are a couple of browsers that pass it by half, work with the ads they have different, and use them unusually and uncomfortably.</t>
+    <t>😩. Changes pleased, using the chanterelle is now much more convenient, the only thing, the variability of the type of tabs should still be (freedom is conservative). I would very much like to have an ad blocker inside the browser that would pass the check of the checkbox, there are a couple of browsers that pass it by half, work with the ads they have different, and use them unusually and uncomfortably.</t>
   </si>
   <si>
     <t>Improved!. I still have to improve the resolution of the Google logo when doing searches .... that&amp;#39;s what bothers me about Safari</t>
@@ -909,7 +1036,7 @@
     <t>Bester Browser. My favorite browser on all systems. Comes chic and powerful therefore. I just need an AdBlocker add-on. Unfortunately, he still does not support self-paced sync servers, really a shame ...</t>
   </si>
   <si>
-    <t>Top App. I really like the new design_ÙÔ_ÙÈ The app is easy to use and runs smoothly.</t>
+    <t>Top App. I really like the new design👍🏻 The app is easy to use and runs smoothly.</t>
   </si>
   <si>
     <t>Bad .... - Possibly, the new UI even worse than the old - bookmark management pathetic - sluggish and slow - even on the Mozilla side already misrepresentations - unsolicited, unwanted and not turn off &amp;quot;recommendations&amp;quot; do not go !! Mozilla is slowly getting rid of himself. Both the apps and the desktop versions. If only the safari were not worse ... :(</t>
@@ -936,7 +1063,7 @@
     <t>Flick&amp;#39;s reaction. The brick operation of the forward and return must move the finger greatly from the edge, and it feels stressed. I want you to change so that it reacts not by position but by operation.</t>
   </si>
   <si>
-    <t>Excellent. I love the Firefox project! This update is perfect for me likes! Combine everything good! And the most important thing is that it is safer and more private! _ÙÔ</t>
+    <t>Excellent. I love the Firefox project! This update is perfect for me likes! Combine everything good! And the most important thing is that it is safer and more private! 👍</t>
   </si>
   <si>
     <t>Perfect. It is the most used app I have, it is just perfect and the new style that was given is beautiful. Very good job, congratulations, keep it up.</t>
@@ -945,7 +1072,7 @@
     <t>New icon. Make the background of the icon lighter.</t>
   </si>
   <si>
-    <t>Very fast. This new update is fast than a bullet Congratulations _ÙÔ_ÙÔ_ÙÔ Mozilla Just missing a black theme in the App.</t>
+    <t>Very fast. This new update is fast than a bullet Congratulations 👏👏👏 Mozilla Just missing a black theme in the App.</t>
   </si>
   <si>
     <t>Actually do not block ads. Actually not screened ads actually not screened ads actually not screened ads</t>
@@ -972,7 +1099,7 @@
     <t>Terrible!. Change the background of the icon: remove the black !!! And make search engine suggestions turn-off: brakes terribly !!!</t>
   </si>
   <si>
-    <t>Supeerr. The best browser I use is _ÙÔ</t>
+    <t>Supeerr. The best browser I use is 👍</t>
   </si>
   <si>
     <t>About Night mode. Hope that after opening the night mode, bookmarks and history can also be a night theme, the other okay, support</t>
@@ -1017,15 +1144,15 @@
     <t>Great Browser!. Photon now has more gear! Very beautifull! Bravi! I look forward to the desktop version next week :) W Mozilla!</t>
   </si>
   <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
     <t>Negative</t>
   </si>
   <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Neutral</t>
-  </si>
-  <si>
     <t>Bookmark, Firefox/Browser/App</t>
   </si>
   <si>
@@ -1500,22 +1627,22 @@
     <t>Clear, Crash</t>
   </si>
   <si>
-    <t>updat, ad, ûªt</t>
-  </si>
-  <si>
-    <t>ûªs, improv, set, option, load, chang, allow, menu</t>
-  </si>
-  <si>
-    <t>updat, mozilla, final, interfac, fast, bar, menu</t>
-  </si>
-  <si>
-    <t>chrome, ûªs, improv, ûªt, googl, bar, button, data</t>
+    <t>updat, ad</t>
+  </si>
+  <si>
+    <t>improv, set, option, load, chang, allow, menu</t>
+  </si>
+  <si>
+    <t>updat, mozilla, final, interfac, fast, bar, photon, menu</t>
+  </si>
+  <si>
+    <t>chrome, improv, googl, bar, button, data</t>
   </si>
   <si>
     <t>load, data</t>
   </si>
   <si>
-    <t>look, ûªs</t>
+    <t>look</t>
   </si>
   <si>
     <t>design</t>
@@ -1530,99 +1657,99 @@
     <t>add</t>
   </si>
   <si>
+    <t>ad, mozilla, ui</t>
+  </si>
+  <si>
+    <t>updat, final</t>
+  </si>
+  <si>
+    <t>improv, interfac, add</t>
+  </si>
+  <si>
+    <t>ad, add</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>updat, chrome, googl</t>
+  </si>
+  <si>
+    <t>updat</t>
+  </si>
+  <si>
+    <t>bar, button, menu</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>design, photon</t>
+  </si>
+  <si>
+    <t>updat, look, ad, googl, photon</t>
+  </si>
+  <si>
+    <t>featur, websit</t>
+  </si>
+  <si>
+    <t>bar, menu</t>
+  </si>
+  <si>
+    <t>updat, switch</t>
+  </si>
+  <si>
+    <t>design, fast</t>
+  </si>
+  <si>
+    <t>updat, load, close</t>
+  </si>
+  <si>
+    <t>option, chang</t>
+  </si>
+  <si>
+    <t>look, icon, option, load, background, websit, black, menu</t>
+  </si>
+  <si>
+    <t>look, set, option, chang, button</t>
+  </si>
+  <si>
+    <t>option, mozilla, design</t>
+  </si>
+  <si>
+    <t>featur, button, photon, data</t>
+  </si>
+  <si>
+    <t>updat, photon, websit</t>
+  </si>
+  <si>
+    <t>updat, look</t>
+  </si>
+  <si>
+    <t>updat, fast</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
+    <t>look, icon, background, black</t>
+  </si>
+  <si>
+    <t>featur, ad, set, data</t>
+  </si>
+  <si>
+    <t>look, featur, websit</t>
+  </si>
+  <si>
+    <t>updat, googl</t>
+  </si>
+  <si>
     <t>ad, mozilla</t>
   </si>
   <si>
-    <t>updat, final</t>
-  </si>
-  <si>
-    <t>improv, interfac, add</t>
-  </si>
-  <si>
-    <t>ad, add</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>updat, chrome, ûªt, googl</t>
-  </si>
-  <si>
-    <t>updat</t>
-  </si>
-  <si>
-    <t>bar, button, menu</t>
-  </si>
-  <si>
-    <t>set</t>
-  </si>
-  <si>
-    <t>look</t>
-  </si>
-  <si>
-    <t>updat, look, ûªs, ad, ûªt, googl</t>
-  </si>
-  <si>
-    <t>featur, websit</t>
-  </si>
-  <si>
-    <t>bar, menu</t>
-  </si>
-  <si>
-    <t>updat, switch</t>
-  </si>
-  <si>
-    <t>ûªs, design, fast</t>
-  </si>
-  <si>
-    <t>updat, ûªt, load, close</t>
-  </si>
-  <si>
-    <t>option, chang</t>
-  </si>
-  <si>
-    <t>look, icon, option, load, background, websit, black, menu</t>
-  </si>
-  <si>
-    <t>look, set, option, chang, button</t>
-  </si>
-  <si>
-    <t>option, mozilla, design</t>
-  </si>
-  <si>
-    <t>featur, button, data</t>
-  </si>
-  <si>
-    <t>icon, ûªs</t>
-  </si>
-  <si>
-    <t>updat, websit</t>
-  </si>
-  <si>
-    <t>updat, look</t>
-  </si>
-  <si>
-    <t>updat, fast</t>
-  </si>
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>background</t>
-  </si>
-  <si>
-    <t>look, icon, background, black</t>
-  </si>
-  <si>
-    <t>featur, ad, set, data</t>
-  </si>
-  <si>
-    <t>look, featur, websit</t>
-  </si>
-  <si>
-    <t>updat, ûªt, googl</t>
-  </si>
-  <si>
     <t>updat, look, featur, set, add, load, googl</t>
   </si>
   <si>
@@ -1635,7 +1762,7 @@
     <t>chrome, final, design</t>
   </si>
   <si>
-    <t>updat, look, ûªs, set, mozilla, ûªt, googl, switch, allow, menu</t>
+    <t>updat, look, chrome, set, mozilla, googl, switch, allow, menu</t>
   </si>
   <si>
     <t>chang, bar</t>
@@ -1647,7 +1774,7 @@
     <t>final, load</t>
   </si>
   <si>
-    <t>ûªs, mozilla, websit</t>
+    <t>mozilla, websit</t>
   </si>
   <si>
     <t>updat, load, fast</t>
@@ -1665,7 +1792,7 @@
     <t>updat, set, mozilla</t>
   </si>
   <si>
-    <t>updat, icon, improv, ûªt, final, googl, bar, switch</t>
+    <t>updat, icon, improv, final, googl, bar, switch, ui</t>
   </si>
   <si>
     <t>set, add</t>
@@ -1677,7 +1804,7 @@
     <t>improv, final</t>
   </si>
   <si>
-    <t>updat, ûªs, interfac</t>
+    <t>updat, interfac</t>
   </si>
   <si>
     <t>featur, ad, set, option, design, add, chang, background, switch, close, black</t>
@@ -1686,10 +1813,10 @@
     <t>option, button, menu</t>
   </si>
   <si>
-    <t>ûªt, close</t>
-  </si>
-  <si>
-    <t>chrome, ûªs, design, fast</t>
+    <t>close</t>
+  </si>
+  <si>
+    <t>chrome, design, fast</t>
   </si>
   <si>
     <t>look, interfac</t>
@@ -1701,10 +1828,10 @@
     <t>menu</t>
   </si>
   <si>
-    <t>featur, set, ûªt, add</t>
-  </si>
-  <si>
-    <t>updat, featur, ad, improv, set, option, allow</t>
+    <t>featur, set, add</t>
+  </si>
+  <si>
+    <t>updat, featur, ad, improv, set, option, allow, ui</t>
   </si>
   <si>
     <t>icon, chang</t>
@@ -1719,7 +1846,7 @@
     <t>look, chrome</t>
   </si>
   <si>
-    <t>featur, ûªs, improv, switch</t>
+    <t>featur, improv, switch, photon</t>
   </si>
   <si>
     <t>icon, background, black</t>
@@ -1728,13 +1855,16 @@
     <t>option, mozilla, add</t>
   </si>
   <si>
+    <t>featur, ui</t>
+  </si>
+  <si>
     <t>fast</t>
   </si>
   <si>
     <t>chrome, googl</t>
   </si>
   <si>
-    <t>featur, chrome, ûªt</t>
+    <t>featur, chrome</t>
   </si>
   <si>
     <t>button</t>
@@ -1752,16 +1882,16 @@
     <t>updat, interfac, chang, fast</t>
   </si>
   <si>
-    <t>updat, ûªt, load, bar, close, websit</t>
+    <t>updat, load, bar, close, websit</t>
   </si>
   <si>
     <t>look, improv</t>
   </si>
   <si>
-    <t>updat, ûªs, ûªt, googl, websit</t>
-  </si>
-  <si>
-    <t>chrome, ûªs, option, ûªt, interfac, chang</t>
+    <t>updat, googl, websit</t>
+  </si>
+  <si>
+    <t>chrome, option, interfac, chang</t>
   </si>
   <si>
     <t>ad, chang</t>
@@ -1779,13 +1909,19 @@
     <t>background, black</t>
   </si>
   <si>
+    <t>mozilla, ui</t>
+  </si>
+  <si>
+    <t>updat, featur, ad, improv, set, option, mozilla, final, add, googl, button, switch, allow, photon, websit, ui</t>
+  </si>
+  <si>
     <t>mozilla</t>
   </si>
   <si>
-    <t>updat, featur, ad, improv, set, option, mozilla, final, add, googl, button, switch, allow, websit</t>
-  </si>
-  <si>
-    <t>look, featur, chrome, ad, interfac, bar, button, switch, menu</t>
+    <t>look, photon</t>
+  </si>
+  <si>
+    <t>look, featur, chrome, ad, interfac, bar, button, switch, photon, menu</t>
   </si>
   <si>
     <t>chrome, improv, mozilla, interfac, allow</t>
@@ -1794,33 +1930,33 @@
     <t>updat, final, button</t>
   </si>
   <si>
-    <t>look, featur, chrome, ad, interfac, button, switch</t>
+    <t>look, featur, chrome, ad, interfac, button, switch, photon</t>
   </si>
   <si>
     <t>chang</t>
   </si>
   <si>
-    <t>ûªt</t>
+    <t>chrome, ui</t>
   </si>
   <si>
     <t>updat, chrome, improv, mozilla, final</t>
   </si>
   <si>
-    <t>updat, option, final</t>
+    <t>updat, option, final, ui</t>
   </si>
   <si>
     <t>updat, mozilla, fast, black</t>
   </si>
   <si>
+    <t>ui</t>
+  </si>
+  <si>
     <t>ad</t>
   </si>
   <si>
     <t>mozilla, design</t>
   </si>
   <si>
-    <t>updat, interfac</t>
-  </si>
-  <si>
     <t>option, design, button</t>
   </si>
   <si>
@@ -1830,12 +1966,6 @@
     <t>updat, look, chrome, icon, black</t>
   </si>
   <si>
-    <t>chrome, ûªs</t>
-  </si>
-  <si>
-    <t>updat, look, ûªs</t>
-  </si>
-  <si>
     <t>chrome, fast</t>
   </si>
   <si>
@@ -1851,13 +1981,10 @@
     <t>final, interfac, fast, websit, black, data</t>
   </si>
   <si>
-    <t>ûªs, ûªt</t>
-  </si>
-  <si>
     <t>final, switch</t>
   </si>
   <si>
-    <t>final</t>
+    <t>final, photon</t>
   </si>
   <si>
     <t>improv, option, final</t>
@@ -1866,13 +1993,13 @@
     <t>chang, websit</t>
   </si>
   <si>
-    <t>look, ûªs, ûªt, googl</t>
+    <t>look, googl</t>
   </si>
   <si>
     <t>improv</t>
   </si>
   <si>
-    <t>look, mozilla</t>
+    <t>look, mozilla, photon</t>
   </si>
   <si>
     <t># Reviews</t>
@@ -2566,7 +2693,7 @@
         <v>239</v>
       </c>
       <c r="H7" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I7" t="s">
         <v>341</v>
@@ -2636,7 +2763,7 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I9" t="s">
         <v>337</v>
@@ -2729,7 +2856,7 @@
         <v>241</v>
       </c>
       <c r="H12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I12" t="s">
         <v>342</v>
@@ -2828,7 +2955,7 @@
         <v>26</v>
       </c>
       <c r="H15" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I15" t="s">
         <v>342</v>
@@ -2898,7 +3025,7 @@
         <v>244</v>
       </c>
       <c r="H17" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I17" t="s">
         <v>343</v>
@@ -2994,7 +3121,7 @@
         <v>31</v>
       </c>
       <c r="H20" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I20" t="s">
         <v>342</v>
@@ -3029,7 +3156,7 @@
         <v>32</v>
       </c>
       <c r="H21" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I21" t="s">
         <v>342</v>
@@ -3064,7 +3191,7 @@
         <v>33</v>
       </c>
       <c r="H22" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I22" t="s">
         <v>344</v>
@@ -3134,7 +3261,7 @@
         <v>248</v>
       </c>
       <c r="H24" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I24" t="s">
         <v>342</v>
@@ -3169,7 +3296,7 @@
         <v>36</v>
       </c>
       <c r="H25" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I25" t="s">
         <v>342</v>
@@ -3204,7 +3331,7 @@
         <v>249</v>
       </c>
       <c r="H26" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I26" t="s">
         <v>345</v>
@@ -3245,7 +3372,7 @@
         <v>342</v>
       </c>
       <c r="K27" t="s">
-        <v>500</v>
+        <v>513</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -3277,7 +3404,7 @@
         <v>342</v>
       </c>
       <c r="K28" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -3303,7 +3430,7 @@
         <v>40</v>
       </c>
       <c r="H29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I29" t="s">
         <v>346</v>
@@ -3338,7 +3465,7 @@
         <v>41</v>
       </c>
       <c r="H30" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I30" t="s">
         <v>342</v>
@@ -3370,7 +3497,7 @@
         <v>42</v>
       </c>
       <c r="H31" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I31" t="s">
         <v>342</v>
@@ -3402,7 +3529,7 @@
         <v>43</v>
       </c>
       <c r="H32" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I32" t="s">
         <v>342</v>
@@ -3437,7 +3564,7 @@
         <v>250</v>
       </c>
       <c r="H33" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I33" t="s">
         <v>347</v>
@@ -3536,7 +3663,7 @@
         <v>47</v>
       </c>
       <c r="H36" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I36" t="s">
         <v>348</v>
@@ -3606,7 +3733,7 @@
         <v>251</v>
       </c>
       <c r="H38" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I38" t="s">
         <v>350</v>
@@ -3699,7 +3826,7 @@
         <v>252</v>
       </c>
       <c r="H41" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I41" t="s">
         <v>342</v>
@@ -3766,7 +3893,7 @@
         <v>54</v>
       </c>
       <c r="H43" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I43" t="s">
         <v>353</v>
@@ -3833,7 +3960,7 @@
         <v>56</v>
       </c>
       <c r="H45" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I45" t="s">
         <v>355</v>
@@ -3865,13 +3992,13 @@
         <v>57</v>
       </c>
       <c r="H46" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I46" t="s">
         <v>337</v>
       </c>
       <c r="K46" t="s">
-        <v>525</v>
+        <v>502</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -3897,7 +4024,7 @@
         <v>58</v>
       </c>
       <c r="H47" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I47" t="s">
         <v>356</v>
@@ -3906,7 +4033,7 @@
         <v>420</v>
       </c>
       <c r="K47" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -3964,7 +4091,7 @@
         <v>60</v>
       </c>
       <c r="H49" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I49" t="s">
         <v>342</v>
@@ -3973,7 +4100,7 @@
         <v>402</v>
       </c>
       <c r="K49" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -3999,7 +4126,7 @@
         <v>61</v>
       </c>
       <c r="H50" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I50" t="s">
         <v>342</v>
@@ -4008,7 +4135,7 @@
         <v>422</v>
       </c>
       <c r="K50" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -4034,7 +4161,7 @@
         <v>254</v>
       </c>
       <c r="H51" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I51" t="s">
         <v>350</v>
@@ -4075,7 +4202,7 @@
         <v>423</v>
       </c>
       <c r="K52" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -4101,7 +4228,7 @@
         <v>64</v>
       </c>
       <c r="H53" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I53" t="s">
         <v>357</v>
@@ -4133,7 +4260,7 @@
         <v>65</v>
       </c>
       <c r="H54" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I54" t="s">
         <v>358</v>
@@ -4142,7 +4269,7 @@
         <v>425</v>
       </c>
       <c r="K54" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -4168,7 +4295,7 @@
         <v>66</v>
       </c>
       <c r="H55" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I55" t="s">
         <v>337</v>
@@ -4197,7 +4324,7 @@
         <v>67</v>
       </c>
       <c r="H56" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I56" t="s">
         <v>342</v>
@@ -4206,7 +4333,7 @@
         <v>426</v>
       </c>
       <c r="K56" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -4241,7 +4368,7 @@
         <v>427</v>
       </c>
       <c r="K57" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -4276,7 +4403,7 @@
         <v>398</v>
       </c>
       <c r="K58" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -4311,7 +4438,7 @@
         <v>402</v>
       </c>
       <c r="K59" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -4346,7 +4473,7 @@
         <v>419</v>
       </c>
       <c r="K60" t="s">
-        <v>504</v>
+        <v>534</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -4372,7 +4499,7 @@
         <v>72</v>
       </c>
       <c r="H61" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I61" t="s">
         <v>360</v>
@@ -4407,7 +4534,7 @@
         <v>257</v>
       </c>
       <c r="H62" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I62" t="s">
         <v>348</v>
@@ -4474,7 +4601,7 @@
         <v>75</v>
       </c>
       <c r="H64" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I64" t="s">
         <v>356</v>
@@ -4509,7 +4636,7 @@
         <v>259</v>
       </c>
       <c r="H65" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I65" t="s">
         <v>342</v>
@@ -4579,7 +4706,7 @@
         <v>260</v>
       </c>
       <c r="H67" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I67" t="s">
         <v>362</v>
@@ -4614,7 +4741,7 @@
         <v>79</v>
       </c>
       <c r="H68" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I68" t="s">
         <v>345</v>
@@ -4652,7 +4779,7 @@
         <v>398</v>
       </c>
       <c r="K69" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -4678,7 +4805,7 @@
         <v>262</v>
       </c>
       <c r="H70" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I70" t="s">
         <v>363</v>
@@ -4809,7 +4936,7 @@
         <v>85</v>
       </c>
       <c r="H74" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I74" t="s">
         <v>364</v>
@@ -4876,7 +5003,7 @@
         <v>87</v>
       </c>
       <c r="H76" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I76" t="s">
         <v>342</v>
@@ -4911,7 +5038,7 @@
         <v>264</v>
       </c>
       <c r="H77" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I77" t="s">
         <v>337</v>
@@ -4975,7 +5102,7 @@
         <v>90</v>
       </c>
       <c r="H79" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I79" t="s">
         <v>348</v>
@@ -5077,7 +5204,7 @@
         <v>266</v>
       </c>
       <c r="H82" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I82" t="s">
         <v>365</v>
@@ -5147,7 +5274,7 @@
         <v>95</v>
       </c>
       <c r="H84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I84" t="s">
         <v>366</v>
@@ -5182,7 +5309,7 @@
         <v>267</v>
       </c>
       <c r="H85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I85" t="s">
         <v>350</v>
@@ -5287,7 +5414,7 @@
         <v>99</v>
       </c>
       <c r="H88" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I88" t="s">
         <v>342</v>
@@ -5354,7 +5481,7 @@
         <v>101</v>
       </c>
       <c r="H90" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I90" t="s">
         <v>367</v>
@@ -5389,7 +5516,7 @@
         <v>102</v>
       </c>
       <c r="H91" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I91" t="s">
         <v>353</v>
@@ -5424,13 +5551,13 @@
         <v>268</v>
       </c>
       <c r="H92" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I92" t="s">
         <v>337</v>
       </c>
       <c r="K92" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -5456,7 +5583,7 @@
         <v>104</v>
       </c>
       <c r="H93" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I93" t="s">
         <v>368</v>
@@ -5488,7 +5615,7 @@
         <v>105</v>
       </c>
       <c r="H94" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I94" t="s">
         <v>342</v>
@@ -5523,7 +5650,7 @@
         <v>106</v>
       </c>
       <c r="H95" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I95" t="s">
         <v>369</v>
@@ -5558,7 +5685,7 @@
         <v>107</v>
       </c>
       <c r="H96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I96" t="s">
         <v>360</v>
@@ -5625,7 +5752,7 @@
         <v>109</v>
       </c>
       <c r="H98" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I98" t="s">
         <v>337</v>
@@ -5686,7 +5813,7 @@
         <v>270</v>
       </c>
       <c r="H100" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I100" t="s">
         <v>337</v>
@@ -5718,7 +5845,7 @@
         <v>271</v>
       </c>
       <c r="H101" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I101" t="s">
         <v>347</v>
@@ -5753,7 +5880,7 @@
         <v>113</v>
       </c>
       <c r="H102" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I102" t="s">
         <v>347</v>
@@ -5782,7 +5909,7 @@
         <v>272</v>
       </c>
       <c r="H103" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I103" t="s">
         <v>353</v>
@@ -5884,7 +6011,7 @@
         <v>117</v>
       </c>
       <c r="H106" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I106" t="s">
         <v>342</v>
@@ -5954,7 +6081,7 @@
         <v>273</v>
       </c>
       <c r="H108" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I108" t="s">
         <v>355</v>
@@ -6021,7 +6148,7 @@
         <v>274</v>
       </c>
       <c r="H110" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I110" t="s">
         <v>342</v>
@@ -6056,7 +6183,7 @@
         <v>122</v>
       </c>
       <c r="H111" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I111" t="s">
         <v>342</v>
@@ -6091,7 +6218,7 @@
         <v>275</v>
       </c>
       <c r="H112" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I112" t="s">
         <v>354</v>
@@ -6126,7 +6253,7 @@
         <v>276</v>
       </c>
       <c r="H113" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I113" t="s">
         <v>348</v>
@@ -6158,7 +6285,7 @@
         <v>277</v>
       </c>
       <c r="H114" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I114" t="s">
         <v>372</v>
@@ -6222,7 +6349,7 @@
         <v>127</v>
       </c>
       <c r="H116" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I116" t="s">
         <v>342</v>
@@ -6283,7 +6410,7 @@
         <v>279</v>
       </c>
       <c r="H118" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I118" t="s">
         <v>339</v>
@@ -6327,7 +6454,7 @@
         <v>407</v>
       </c>
       <c r="K119" t="s">
-        <v>545</v>
+        <v>570</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -6362,7 +6489,7 @@
         <v>405</v>
       </c>
       <c r="K120" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="121" spans="1:11">
@@ -6388,7 +6515,7 @@
         <v>132</v>
       </c>
       <c r="H121" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I121" t="s">
         <v>373</v>
@@ -6397,7 +6524,7 @@
         <v>456</v>
       </c>
       <c r="K121" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="122" spans="1:11">
@@ -6423,7 +6550,7 @@
         <v>280</v>
       </c>
       <c r="H122" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I122" t="s">
         <v>374</v>
@@ -6455,7 +6582,7 @@
         <v>134</v>
       </c>
       <c r="H123" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I123" t="s">
         <v>342</v>
@@ -6487,7 +6614,7 @@
         <v>281</v>
       </c>
       <c r="H124" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I124" t="s">
         <v>375</v>
@@ -6525,7 +6652,7 @@
         <v>458</v>
       </c>
       <c r="K125" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="126" spans="1:11">
@@ -6557,7 +6684,7 @@
         <v>337</v>
       </c>
       <c r="K126" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
     </row>
     <row r="127" spans="1:11">
@@ -6583,7 +6710,7 @@
         <v>282</v>
       </c>
       <c r="H127" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I127" t="s">
         <v>342</v>
@@ -6627,7 +6754,7 @@
         <v>398</v>
       </c>
       <c r="K128" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
     </row>
     <row r="129" spans="1:11">
@@ -6653,7 +6780,7 @@
         <v>140</v>
       </c>
       <c r="H129" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I129" t="s">
         <v>342</v>
@@ -6662,7 +6789,7 @@
         <v>459</v>
       </c>
       <c r="K129" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="130" spans="1:11">
@@ -6688,7 +6815,7 @@
         <v>141</v>
       </c>
       <c r="H130" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I130" t="s">
         <v>360</v>
@@ -6723,7 +6850,7 @@
         <v>142</v>
       </c>
       <c r="H131" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I131" t="s">
         <v>376</v>
@@ -6732,7 +6859,7 @@
         <v>460</v>
       </c>
       <c r="K131" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="132" spans="1:11">
@@ -6790,7 +6917,7 @@
         <v>144</v>
       </c>
       <c r="H133" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I133" t="s">
         <v>342</v>
@@ -6799,7 +6926,7 @@
         <v>461</v>
       </c>
       <c r="K133" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="134" spans="1:11">
@@ -6834,7 +6961,7 @@
         <v>402</v>
       </c>
       <c r="K134" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="135" spans="1:11">
@@ -6904,7 +7031,7 @@
         <v>462</v>
       </c>
       <c r="K136" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="137" spans="1:11">
@@ -6965,7 +7092,7 @@
         <v>149</v>
       </c>
       <c r="H138" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I138" t="s">
         <v>348</v>
@@ -6974,7 +7101,7 @@
         <v>463</v>
       </c>
       <c r="K138" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="139" spans="1:11">
@@ -7000,7 +7127,7 @@
         <v>287</v>
       </c>
       <c r="H139" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I139" t="s">
         <v>342</v>
@@ -7032,7 +7159,7 @@
         <v>288</v>
       </c>
       <c r="H140" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I140" t="s">
         <v>342</v>
@@ -7041,7 +7168,7 @@
         <v>398</v>
       </c>
       <c r="K140" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="141" spans="1:11">
@@ -7134,7 +7261,7 @@
         <v>154</v>
       </c>
       <c r="H143" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I143" t="s">
         <v>342</v>
@@ -7143,7 +7270,7 @@
         <v>466</v>
       </c>
       <c r="K143" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="144" spans="1:11">
@@ -7169,7 +7296,7 @@
         <v>290</v>
       </c>
       <c r="H144" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I144" t="s">
         <v>342</v>
@@ -7198,7 +7325,7 @@
         <v>156</v>
       </c>
       <c r="H145" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I145" t="s">
         <v>377</v>
@@ -7207,7 +7334,7 @@
         <v>467</v>
       </c>
       <c r="K145" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="146" spans="1:11">
@@ -7239,7 +7366,7 @@
         <v>337</v>
       </c>
       <c r="K146" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="147" spans="1:11">
@@ -7274,7 +7401,7 @@
         <v>402</v>
       </c>
       <c r="K147" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="148" spans="1:11">
@@ -7309,7 +7436,7 @@
         <v>468</v>
       </c>
       <c r="K148" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="149" spans="1:11">
@@ -7335,7 +7462,7 @@
         <v>293</v>
       </c>
       <c r="H149" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I149" t="s">
         <v>342</v>
@@ -7344,7 +7471,7 @@
         <v>469</v>
       </c>
       <c r="K149" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="150" spans="1:11">
@@ -7370,7 +7497,7 @@
         <v>161</v>
       </c>
       <c r="H150" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I150" t="s">
         <v>378</v>
@@ -7379,7 +7506,7 @@
         <v>470</v>
       </c>
       <c r="K150" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="151" spans="1:11">
@@ -7405,7 +7532,7 @@
         <v>162</v>
       </c>
       <c r="H151" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I151" t="s">
         <v>342</v>
@@ -7414,7 +7541,7 @@
         <v>419</v>
       </c>
       <c r="K151" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="152" spans="1:11">
@@ -7481,7 +7608,7 @@
         <v>472</v>
       </c>
       <c r="K153" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="154" spans="1:11">
@@ -7507,7 +7634,7 @@
         <v>295</v>
       </c>
       <c r="H154" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I154" t="s">
         <v>350</v>
@@ -7582,6 +7709,9 @@
       <c r="J156" t="s">
         <v>407</v>
       </c>
+      <c r="K156" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="157" spans="1:11">
       <c r="A157" t="s">
@@ -7606,13 +7736,13 @@
         <v>298</v>
       </c>
       <c r="H157" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I157" t="s">
         <v>336</v>
       </c>
       <c r="K157" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="158" spans="1:11">
@@ -7647,7 +7777,7 @@
         <v>475</v>
       </c>
       <c r="K158" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="159" spans="1:11">
@@ -7682,7 +7812,7 @@
         <v>405</v>
       </c>
       <c r="K159" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="160" spans="1:11">
@@ -7714,7 +7844,7 @@
         <v>337</v>
       </c>
       <c r="K160" t="s">
-        <v>513</v>
+        <v>591</v>
       </c>
     </row>
     <row r="161" spans="1:11">
@@ -7749,7 +7879,7 @@
         <v>476</v>
       </c>
       <c r="K161" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="162" spans="1:11">
@@ -7775,7 +7905,7 @@
         <v>173</v>
       </c>
       <c r="H162" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I162" t="s">
         <v>337</v>
@@ -7804,7 +7934,7 @@
         <v>174</v>
       </c>
       <c r="H163" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I163" t="s">
         <v>339</v>
@@ -7813,7 +7943,7 @@
         <v>477</v>
       </c>
       <c r="K163" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="164" spans="1:11">
@@ -7839,7 +7969,7 @@
         <v>300</v>
       </c>
       <c r="H164" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I164" t="s">
         <v>342</v>
@@ -7848,7 +7978,7 @@
         <v>405</v>
       </c>
       <c r="K164" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="165" spans="1:11">
@@ -7883,7 +8013,7 @@
         <v>478</v>
       </c>
       <c r="K165" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="166" spans="1:11">
@@ -7909,13 +8039,13 @@
         <v>177</v>
       </c>
       <c r="H166" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I166" t="s">
         <v>337</v>
       </c>
       <c r="K166" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="167" spans="1:11">
@@ -7950,7 +8080,7 @@
         <v>476</v>
       </c>
       <c r="K167" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="168" spans="1:11">
@@ -7976,7 +8106,7 @@
         <v>302</v>
       </c>
       <c r="H168" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I168" t="s">
         <v>342</v>
@@ -8008,7 +8138,7 @@
         <v>180</v>
       </c>
       <c r="H169" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I169" t="s">
         <v>342</v>
@@ -8043,7 +8173,7 @@
         <v>303</v>
       </c>
       <c r="H170" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I170" t="s">
         <v>342</v>
@@ -8113,7 +8243,7 @@
         <v>305</v>
       </c>
       <c r="H172" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I172" t="s">
         <v>342</v>
@@ -8122,7 +8252,7 @@
         <v>415</v>
       </c>
       <c r="K172" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="173" spans="1:11">
@@ -8148,7 +8278,7 @@
         <v>184</v>
       </c>
       <c r="H173" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I173" t="s">
         <v>353</v>
@@ -8156,9 +8286,6 @@
       <c r="J173" t="s">
         <v>480</v>
       </c>
-      <c r="K173" t="s">
-        <v>594</v>
-      </c>
     </row>
     <row r="174" spans="1:11">
       <c r="A174" t="s">
@@ -8256,7 +8383,7 @@
         <v>405</v>
       </c>
       <c r="K176" t="s">
-        <v>508</v>
+        <v>597</v>
       </c>
     </row>
     <row r="177" spans="1:11">
@@ -8291,7 +8418,7 @@
         <v>482</v>
       </c>
       <c r="K177" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="178" spans="1:11">
@@ -8355,7 +8482,7 @@
         <v>337</v>
       </c>
       <c r="K179" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="180" spans="1:11">
@@ -8390,7 +8517,7 @@
         <v>402</v>
       </c>
       <c r="K180" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="181" spans="1:11">
@@ -8425,7 +8552,7 @@
         <v>483</v>
       </c>
       <c r="K181" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="182" spans="1:11">
@@ -8451,7 +8578,7 @@
         <v>193</v>
       </c>
       <c r="H182" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I182" t="s">
         <v>387</v>
@@ -8486,7 +8613,7 @@
         <v>194</v>
       </c>
       <c r="H183" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I183" t="s">
         <v>388</v>
@@ -8494,6 +8621,9 @@
       <c r="J183" t="s">
         <v>485</v>
       </c>
+      <c r="K183" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="184" spans="1:11">
       <c r="A184" t="s">
@@ -8518,13 +8648,13 @@
         <v>310</v>
       </c>
       <c r="H184" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I184" t="s">
         <v>337</v>
       </c>
       <c r="K184" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
     </row>
     <row r="185" spans="1:11">
@@ -8591,7 +8721,7 @@
         <v>486</v>
       </c>
       <c r="K186" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
     </row>
     <row r="187" spans="1:11">
@@ -8617,7 +8747,7 @@
         <v>313</v>
       </c>
       <c r="H187" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I187" t="s">
         <v>353</v>
@@ -8681,7 +8811,7 @@
         <v>315</v>
       </c>
       <c r="H189" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I189" t="s">
         <v>342</v>
@@ -8690,7 +8820,7 @@
         <v>481</v>
       </c>
       <c r="K189" t="s">
-        <v>600</v>
+        <v>553</v>
       </c>
     </row>
     <row r="190" spans="1:11">
@@ -8716,7 +8846,7 @@
         <v>316</v>
       </c>
       <c r="H190" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I190" t="s">
         <v>336</v>
@@ -8725,7 +8855,7 @@
         <v>398</v>
       </c>
       <c r="K190" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="191" spans="1:11">
@@ -8751,7 +8881,7 @@
         <v>317</v>
       </c>
       <c r="H191" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I191" t="s">
         <v>389</v>
@@ -8760,7 +8890,7 @@
         <v>487</v>
       </c>
       <c r="K191" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="192" spans="1:11">
@@ -8786,7 +8916,7 @@
         <v>203</v>
       </c>
       <c r="H192" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I192" t="s">
         <v>353</v>
@@ -8847,7 +8977,7 @@
         <v>319</v>
       </c>
       <c r="H194" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I194" t="s">
         <v>390</v>
@@ -8879,7 +9009,7 @@
         <v>320</v>
       </c>
       <c r="H195" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I195" t="s">
         <v>342</v>
@@ -8888,7 +9018,7 @@
         <v>402</v>
       </c>
       <c r="K195" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="196" spans="1:11">
@@ -8920,7 +9050,7 @@
         <v>342</v>
       </c>
       <c r="K196" t="s">
-        <v>604</v>
+        <v>508</v>
       </c>
     </row>
     <row r="197" spans="1:11">
@@ -8946,7 +9076,7 @@
         <v>321</v>
       </c>
       <c r="H197" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I197" t="s">
         <v>342</v>
@@ -9022,7 +9152,7 @@
         <v>481</v>
       </c>
       <c r="K199" t="s">
-        <v>605</v>
+        <v>526</v>
       </c>
     </row>
     <row r="200" spans="1:11">
@@ -9054,7 +9184,7 @@
         <v>342</v>
       </c>
       <c r="K200" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="201" spans="1:11">
@@ -9124,7 +9254,7 @@
         <v>403</v>
       </c>
       <c r="K202" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="203" spans="1:11">
@@ -9179,7 +9309,7 @@
         <v>215</v>
       </c>
       <c r="H204" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I204" t="s">
         <v>391</v>
@@ -9188,7 +9318,7 @@
         <v>488</v>
       </c>
       <c r="K204" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="205" spans="1:11">
@@ -9214,7 +9344,7 @@
         <v>325</v>
       </c>
       <c r="H205" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I205" t="s">
         <v>337</v>
@@ -9278,7 +9408,7 @@
         <v>218</v>
       </c>
       <c r="H207" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I207" t="s">
         <v>342</v>
@@ -9319,7 +9449,7 @@
         <v>482</v>
       </c>
       <c r="K208" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="209" spans="1:11">
@@ -9354,7 +9484,7 @@
         <v>401</v>
       </c>
       <c r="K209" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="210" spans="1:11">
@@ -9380,7 +9510,7 @@
         <v>221</v>
       </c>
       <c r="H210" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I210" t="s">
         <v>345</v>
@@ -9388,9 +9518,6 @@
       <c r="J210" t="s">
         <v>407</v>
       </c>
-      <c r="K210" t="s">
-        <v>611</v>
-      </c>
     </row>
     <row r="211" spans="1:11">
       <c r="A211" t="s">
@@ -9415,7 +9542,7 @@
         <v>326</v>
       </c>
       <c r="H211" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I211" t="s">
         <v>350</v>
@@ -9587,7 +9714,7 @@
         <v>227</v>
       </c>
       <c r="H216" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I216" t="s">
         <v>354</v>
@@ -9619,7 +9746,7 @@
         <v>228</v>
       </c>
       <c r="H217" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I217" t="s">
         <v>358</v>
@@ -9627,9 +9754,6 @@
       <c r="J217" t="s">
         <v>425</v>
       </c>
-      <c r="K217" t="s">
-        <v>594</v>
-      </c>
     </row>
     <row r="218" spans="1:11">
       <c r="A218" t="s">
@@ -9750,14 +9874,11 @@
         <v>232</v>
       </c>
       <c r="H221" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I221" t="s">
         <v>337</v>
       </c>
-      <c r="K221" t="s">
-        <v>594</v>
-      </c>
     </row>
     <row r="222" spans="1:11">
       <c r="A222" t="s">
@@ -9826,7 +9947,7 @@
         <v>493</v>
       </c>
       <c r="K223" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="224" spans="1:11">
@@ -9852,7 +9973,7 @@
         <v>235</v>
       </c>
       <c r="H224" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I224" t="s">
         <v>342</v>

</xml_diff>